<commit_message>
patch para caso nulo de dados de labor
</commit_message>
<xml_diff>
--- a/arquivos/SIEGE-ORCAMENTO-ID_99.xlsx
+++ b/arquivos/SIEGE-ORCAMENTO-ID_99.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="#0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="##0.00"/>
@@ -27,8 +27,9 @@
     <numFmt numFmtId="168" formatCode="#,##0.0000"/>
     <numFmt numFmtId="169" formatCode="##,##0.00"/>
     <numFmt numFmtId="170" formatCode="###,##0.00"/>
+    <numFmt numFmtId="171" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -60,6 +61,11 @@
       <color theme="0"/>
       <sz val="16"/>
       <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -197,10 +203,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -290,6 +297,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="171" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -302,6 +317,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="170" fontId="3" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="170" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -325,8 +346,9 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors/>
@@ -334,7 +356,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -352,24 +374,24 @@
       <nvPicPr>
         <cNvPr id="3" name="Imagem 2"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="66676" y="53340"/>
           <a:ext cx="1543243" cy="758190"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -380,7 +402,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -398,24 +420,24 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagem 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="66676" y="53340"/>
           <a:ext cx="1545148" cy="758190"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -426,7 +448,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -444,24 +466,24 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagem 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="66676" y="53340"/>
           <a:ext cx="1545148" cy="758190"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -472,7 +494,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -490,24 +512,24 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagem 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="66676" y="53340"/>
           <a:ext cx="1545148" cy="758190"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -518,7 +540,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>0</col>
@@ -536,24 +558,24 @@
       <nvPicPr>
         <cNvPr id="2" name="Imagem 1"/>
         <cNvPicPr>
-          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </cNvPicPr>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="66676" y="53340"/>
           <a:ext cx="1545148" cy="758190"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -859,7 +881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -867,7 +889,7 @@
   <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="10.2"/>
@@ -876,41 +898,41 @@
     <col width="58.109375" customWidth="1" style="1" min="2" max="2"/>
     <col width="12" customWidth="1" style="1" min="3" max="3"/>
     <col width="9.5546875" customWidth="1" style="1" min="4" max="4"/>
-    <col width="11.33203125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="12.109375" customWidth="1" style="1" min="6" max="6"/>
-    <col width="17.88671875" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
-    <col width="16.109375" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="11.33203125" customWidth="1" style="34" min="5" max="5"/>
+    <col width="12.109375" customWidth="1" style="34" min="6" max="6"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="34" min="7" max="7"/>
+    <col width="16.109375" bestFit="1" customWidth="1" style="34" min="8" max="8"/>
     <col width="1.44140625" bestFit="1" customWidth="1" style="1" min="9" max="9"/>
     <col width="9.109375" customWidth="1" style="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>PLANILHA ORÇAMENTÁRIA</t>
         </is>
       </c>
-      <c r="B1" s="32" t="n"/>
-      <c r="C1" s="32" t="n"/>
-      <c r="D1" s="32" t="n"/>
-      <c r="E1" s="32" t="n"/>
-      <c r="F1" s="32" t="n"/>
-      <c r="G1" s="32" t="n"/>
-      <c r="H1" s="33" t="n"/>
+      <c r="B1" s="36" t="n"/>
+      <c r="C1" s="36" t="n"/>
+      <c r="D1" s="36" t="n"/>
+      <c r="E1" s="36" t="n"/>
+      <c r="F1" s="36" t="n"/>
+      <c r="G1" s="36" t="n"/>
+      <c r="H1" s="37" t="n"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="34" t="n"/>
-      <c r="H2" s="35" t="n"/>
+      <c r="A2" s="38" t="n"/>
+      <c r="H2" s="39" t="n"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="36" t="n"/>
-      <c r="B3" s="37" t="n"/>
-      <c r="C3" s="37" t="n"/>
-      <c r="D3" s="37" t="n"/>
-      <c r="E3" s="37" t="n"/>
-      <c r="F3" s="37" t="n"/>
-      <c r="G3" s="37" t="n"/>
-      <c r="H3" s="38" t="n"/>
+      <c r="A3" s="40" t="n"/>
+      <c r="B3" s="41" t="n"/>
+      <c r="C3" s="41" t="n"/>
+      <c r="D3" s="41" t="n"/>
+      <c r="E3" s="41" t="n"/>
+      <c r="F3" s="41" t="n"/>
+      <c r="G3" s="41" t="n"/>
+      <c r="H3" s="42" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
@@ -928,7 +950,10 @@
           <t>Obra</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n"/>
+      <c r="B5" s="5">
+        <f>B12</f>
+        <v/>
+      </c>
       <c r="C5" s="5" t="n"/>
       <c r="D5" s="5" t="n"/>
       <c r="E5" s="5" t="n"/>
@@ -967,8 +992,15 @@
       <c r="D8" s="4" t="n"/>
       <c r="E8" s="8" t="n"/>
       <c r="F8" s="8" t="n"/>
-      <c r="G8" s="8" t="n"/>
-      <c r="H8" s="39" t="n"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="H8" s="43">
+        <f>SUM(H12:H1048576)</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
@@ -978,10 +1010,12 @@
       <c r="E9" s="8" t="n"/>
       <c r="F9" s="8" t="n"/>
       <c r="G9" s="8" t="n"/>
-      <c r="H9" s="39" t="n"/>
+      <c r="H9" s="43" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="21" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -1038,12 +1072,14 @@
       </c>
       <c r="C12" s="9" t="n"/>
       <c r="D12" s="10" t="n"/>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="10" t="n"/>
-      <c r="G12" s="10" t="n"/>
-      <c r="H12" s="40" t="n"/>
+      <c r="F12" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="44" t="n"/>
+      <c r="H12" s="44" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="20" t="inlineStr">
@@ -1058,12 +1094,14 @@
       </c>
       <c r="C13" s="9" t="n"/>
       <c r="D13" s="10" t="n"/>
-      <c r="E13" s="10" t="n">
+      <c r="E13" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="10" t="n"/>
-      <c r="G13" s="10" t="n"/>
-      <c r="H13" s="15" t="n"/>
+      <c r="F13" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="44" t="n"/>
+      <c r="H13" s="44" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="inlineStr">
@@ -1084,16 +1122,16 @@
       <c r="D14" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="E14" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="44" t="n">
+        <v>51000</v>
+      </c>
+      <c r="G14" s="44" t="n">
         <v>30000</v>
       </c>
-      <c r="G14" s="41" t="n">
-        <v>30000</v>
-      </c>
-      <c r="H14" s="42" t="n">
+      <c r="H14" s="44" t="n">
         <v>30000</v>
       </c>
     </row>
@@ -1116,16 +1154,16 @@
       <c r="D15" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="E15" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="44" t="n">
+        <v>396.1</v>
+      </c>
+      <c r="G15" s="44" t="n">
         <v>233</v>
       </c>
-      <c r="G15" s="43" t="n">
-        <v>233</v>
-      </c>
-      <c r="H15" s="15" t="n">
+      <c r="H15" s="44" t="n">
         <v>233</v>
       </c>
     </row>
@@ -1148,13 +1186,13 @@
       <c r="D16" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="E16" s="44" t="n">
         <v>33.43</v>
       </c>
-      <c r="F16" s="10" t="n">
-        <v>254.2222</v>
-      </c>
-      <c r="G16" s="10" t="n">
+      <c r="F16" s="44" t="n">
+        <v>432.17774</v>
+      </c>
+      <c r="G16" s="44" t="n">
         <v>287.6522</v>
       </c>
       <c r="H16" s="44" t="n">
@@ -1180,16 +1218,16 @@
       <c r="D17" s="10" t="n">
         <v>102.06</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="44" t="n">
         <v>13.4514</v>
       </c>
-      <c r="F17" s="10" t="n">
-        <v>146.4476</v>
-      </c>
-      <c r="G17" s="45" t="n">
+      <c r="F17" s="44" t="n">
+        <v>248.96092</v>
+      </c>
+      <c r="G17" s="44" t="n">
         <v>159.899</v>
       </c>
-      <c r="H17" s="15" t="n">
+      <c r="H17" s="44" t="n">
         <v>16319.29</v>
       </c>
     </row>
@@ -1212,16 +1250,16 @@
       <c r="D18" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="E18" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="F18" s="44" t="n">
+        <v>48552</v>
+      </c>
+      <c r="G18" s="44" t="n">
         <v>28560</v>
       </c>
-      <c r="G18" s="41" t="n">
-        <v>28560</v>
-      </c>
-      <c r="H18" s="15" t="n">
+      <c r="H18" s="44" t="n">
         <v>28560</v>
       </c>
     </row>
@@ -1244,16 +1282,16 @@
       <c r="D19" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="10" t="n">
+      <c r="E19" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="44" t="n">
+        <v>9690</v>
+      </c>
+      <c r="G19" s="44" t="n">
         <v>5700</v>
       </c>
-      <c r="G19" s="43" t="n">
-        <v>5700</v>
-      </c>
-      <c r="H19" s="15" t="n">
+      <c r="H19" s="44" t="n">
         <v>5700</v>
       </c>
     </row>
@@ -1270,12 +1308,14 @@
       </c>
       <c r="C20" s="9" t="n"/>
       <c r="D20" s="10" t="n"/>
-      <c r="E20" s="10" t="n">
+      <c r="E20" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="10" t="n"/>
-      <c r="G20" s="43" t="n"/>
-      <c r="H20" s="15" t="n"/>
+      <c r="F20" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="44" t="n"/>
+      <c r="H20" s="44" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="9" t="inlineStr">
@@ -1296,16 +1336,16 @@
       <c r="D21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="44" t="n">
         <v>595.444</v>
       </c>
-      <c r="F21" s="46" t="n">
-        <v>519.5441000000001</v>
-      </c>
-      <c r="G21" s="46" t="n">
+      <c r="F21" s="44" t="n">
+        <v>883.2249700000001</v>
+      </c>
+      <c r="G21" s="44" t="n">
         <v>1114.9881</v>
       </c>
-      <c r="H21" s="15" t="n">
+      <c r="H21" s="44" t="n">
         <v>1114.98</v>
       </c>
     </row>
@@ -1328,13 +1368,13 @@
       <c r="D22" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="10" t="n">
+      <c r="E22" s="44" t="n">
         <v>10897.5279</v>
       </c>
-      <c r="F22" s="10" t="n">
-        <v>7070.120100000002</v>
-      </c>
-      <c r="G22" s="10" t="n">
+      <c r="F22" s="44" t="n">
+        <v>12019.20417</v>
+      </c>
+      <c r="G22" s="44" t="n">
         <v>17967.648</v>
       </c>
       <c r="H22" s="44" t="n">
@@ -1354,11 +1394,13 @@
       </c>
       <c r="C23" s="9" t="n"/>
       <c r="D23" s="10" t="n"/>
-      <c r="E23" s="10" t="n">
+      <c r="E23" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="10" t="n"/>
-      <c r="G23" s="10" t="n"/>
+      <c r="F23" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="44" t="n"/>
       <c r="H23" s="44" t="n"/>
     </row>
     <row r="24">
@@ -1374,11 +1416,13 @@
       </c>
       <c r="C24" s="9" t="n"/>
       <c r="D24" s="10" t="n"/>
-      <c r="E24" s="10" t="n">
+      <c r="E24" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="10" t="n"/>
-      <c r="G24" s="41" t="n"/>
+      <c r="F24" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="44" t="n"/>
       <c r="H24" s="44" t="n"/>
     </row>
     <row r="25">
@@ -1400,16 +1444,16 @@
       <c r="D25" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E25" s="45" t="n">
+      <c r="E25" s="44" t="n">
         <v>2957.132</v>
       </c>
-      <c r="F25" s="45" t="n">
+      <c r="F25" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="45" t="n">
+      <c r="G25" s="44" t="n">
         <v>2957.132</v>
       </c>
-      <c r="H25" s="42" t="n">
+      <c r="H25" s="44" t="n">
         <v>8871.4</v>
       </c>
     </row>
@@ -1426,12 +1470,14 @@
       </c>
       <c r="C26" s="9" t="n"/>
       <c r="D26" s="10" t="n"/>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="10" t="n"/>
-      <c r="G26" s="41" t="n"/>
-      <c r="H26" s="15" t="n"/>
+      <c r="F26" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="44" t="n"/>
+      <c r="H26" s="44" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="9" t="inlineStr">
@@ -1452,16 +1498,16 @@
       <c r="D27" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="44" t="n">
         <v>10429.28</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="41" t="n">
+      <c r="G27" s="44" t="n">
         <v>10429.28</v>
       </c>
-      <c r="H27" s="15" t="n">
+      <c r="H27" s="44" t="n">
         <v>31287.84</v>
       </c>
     </row>
@@ -1484,16 +1530,16 @@
       <c r="D28" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E28" s="10" t="n">
+      <c r="E28" s="44" t="n">
         <v>7749.12</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="41" t="n">
+      <c r="G28" s="44" t="n">
         <v>7749.12</v>
       </c>
-      <c r="H28" s="15" t="n">
+      <c r="H28" s="44" t="n">
         <v>23247.36</v>
       </c>
     </row>
@@ -1516,16 +1562,16 @@
       <c r="D29" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="44" t="n">
         <v>2092.74</v>
       </c>
-      <c r="F29" s="41" t="n">
+      <c r="F29" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="41" t="n">
+      <c r="G29" s="44" t="n">
         <v>2092.74</v>
       </c>
-      <c r="H29" s="15" t="n">
+      <c r="H29" s="44" t="n">
         <v>6278.22</v>
       </c>
     </row>
@@ -1548,13 +1594,13 @@
       <c r="D30" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="E30" s="10" t="n">
+      <c r="E30" s="44" t="n">
         <v>2921.85</v>
       </c>
-      <c r="F30" s="41" t="n">
+      <c r="F30" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="41" t="n">
+      <c r="G30" s="44" t="n">
         <v>2921.85</v>
       </c>
       <c r="H30" s="44" t="n">
@@ -1574,12 +1620,14 @@
       </c>
       <c r="C31" s="9" t="n"/>
       <c r="D31" s="10" t="n"/>
-      <c r="E31" s="10" t="n">
+      <c r="E31" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F31" s="10" t="n"/>
-      <c r="G31" s="41" t="n"/>
-      <c r="H31" s="15" t="n"/>
+      <c r="F31" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="44" t="n"/>
+      <c r="H31" s="44" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="9" t="inlineStr">
@@ -1600,16 +1648,16 @@
       <c r="D32" s="10" t="n">
         <v>170.66</v>
       </c>
-      <c r="E32" s="10" t="n">
+      <c r="E32" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F32" s="10" t="n">
+      <c r="F32" s="44" t="n">
+        <v>6.867999999999999</v>
+      </c>
+      <c r="G32" s="44" t="n">
         <v>4.04</v>
       </c>
-      <c r="G32" s="41" t="n">
-        <v>4.04</v>
-      </c>
-      <c r="H32" s="15" t="n">
+      <c r="H32" s="44" t="n">
         <v>689.47</v>
       </c>
     </row>
@@ -1632,13 +1680,13 @@
       <c r="D33" s="10" t="n">
         <v>3880</v>
       </c>
-      <c r="E33" s="10" t="n">
+      <c r="E33" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F33" s="10" t="n">
-        <v>28</v>
-      </c>
-      <c r="G33" s="10" t="n">
+      <c r="F33" s="44" t="n">
+        <v>47.6</v>
+      </c>
+      <c r="G33" s="44" t="n">
         <v>28</v>
       </c>
       <c r="H33" s="44" t="n">
@@ -1664,16 +1712,16 @@
       <c r="D34" s="10" t="n">
         <v>3880</v>
       </c>
-      <c r="E34" s="10" t="n">
+      <c r="E34" s="44" t="n">
         <v>3.4357</v>
       </c>
-      <c r="F34" s="10" t="n">
-        <v>2.7368</v>
-      </c>
-      <c r="G34" s="43" t="n">
+      <c r="F34" s="44" t="n">
+        <v>4.65256</v>
+      </c>
+      <c r="G34" s="44" t="n">
         <v>6.1725</v>
       </c>
-      <c r="H34" s="42" t="n">
+      <c r="H34" s="44" t="n">
         <v>23949.3</v>
       </c>
     </row>
@@ -1690,12 +1738,14 @@
       </c>
       <c r="C35" s="9" t="n"/>
       <c r="D35" s="10" t="n"/>
-      <c r="E35" s="43" t="n">
+      <c r="E35" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F35" s="10" t="n"/>
-      <c r="G35" s="43" t="n"/>
-      <c r="H35" s="15" t="n"/>
+      <c r="F35" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="44" t="n"/>
+      <c r="H35" s="44" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="9" t="inlineStr">
@@ -1716,16 +1766,16 @@
       <c r="D36" s="10" t="n">
         <v>147</v>
       </c>
-      <c r="E36" s="46" t="n">
+      <c r="E36" s="44" t="n">
         <v>73.2927</v>
       </c>
-      <c r="F36" s="10" t="n">
-        <v>1327.6462</v>
-      </c>
-      <c r="G36" s="46" t="n">
+      <c r="F36" s="44" t="n">
+        <v>2256.99854</v>
+      </c>
+      <c r="G36" s="44" t="n">
         <v>1400.9389</v>
       </c>
-      <c r="H36" s="15" t="n">
+      <c r="H36" s="44" t="n">
         <v>205938.03</v>
       </c>
     </row>
@@ -1748,16 +1798,16 @@
       <c r="D37" s="10" t="n">
         <v>105</v>
       </c>
-      <c r="E37" s="10" t="n">
+      <c r="E37" s="44" t="n">
         <v>114.3659</v>
       </c>
-      <c r="F37" s="10" t="n">
-        <v>2217.3942</v>
-      </c>
-      <c r="G37" s="46" t="n">
+      <c r="F37" s="44" t="n">
+        <v>3769.57014</v>
+      </c>
+      <c r="G37" s="44" t="n">
         <v>2331.7601</v>
       </c>
-      <c r="H37" s="15" t="n">
+      <c r="H37" s="44" t="n">
         <v>244834.81</v>
       </c>
     </row>
@@ -1780,16 +1830,16 @@
       <c r="D38" s="10" t="n">
         <v>343</v>
       </c>
-      <c r="E38" s="10" t="n">
+      <c r="E38" s="44" t="n">
         <v>7.99</v>
       </c>
-      <c r="F38" s="10" t="n">
-        <v>878.2445</v>
-      </c>
-      <c r="G38" s="43" t="n">
+      <c r="F38" s="44" t="n">
+        <v>1493.01565</v>
+      </c>
+      <c r="G38" s="44" t="n">
         <v>886.2345</v>
       </c>
-      <c r="H38" s="42" t="n">
+      <c r="H38" s="44" t="n">
         <v>303978.43</v>
       </c>
     </row>
@@ -1812,16 +1862,16 @@
       <c r="D39" s="10" t="n">
         <v>245</v>
       </c>
-      <c r="E39" s="43" t="n">
+      <c r="E39" s="44" t="n">
         <v>7.99</v>
       </c>
-      <c r="F39" s="43" t="n">
-        <v>1037.456</v>
-      </c>
-      <c r="G39" s="43" t="n">
+      <c r="F39" s="44" t="n">
+        <v>1763.6752</v>
+      </c>
+      <c r="G39" s="44" t="n">
         <v>1045.446</v>
       </c>
-      <c r="H39" s="42" t="n">
+      <c r="H39" s="44" t="n">
         <v>256134.27</v>
       </c>
     </row>
@@ -1838,12 +1888,14 @@
       </c>
       <c r="C40" s="9" t="n"/>
       <c r="D40" s="10" t="n"/>
-      <c r="E40" s="46" t="n">
+      <c r="E40" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="F40" s="10" t="n"/>
-      <c r="G40" s="46" t="n"/>
-      <c r="H40" s="15" t="n"/>
+      <c r="F40" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="44" t="n"/>
+      <c r="H40" s="44" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="9" t="inlineStr">
@@ -1864,13 +1916,13 @@
       <c r="D41" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E41" s="10" t="n">
+      <c r="E41" s="44" t="n">
         <v>617.65</v>
       </c>
-      <c r="F41" s="10" t="n">
+      <c r="F41" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G41" s="10" t="n">
+      <c r="G41" s="44" t="n">
         <v>617.65</v>
       </c>
       <c r="H41" s="44" t="n">
@@ -1896,13 +1948,13 @@
       <c r="D42" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="E42" s="10" t="n">
+      <c r="E42" s="44" t="n">
         <v>1347.6</v>
       </c>
-      <c r="F42" s="10" t="n">
+      <c r="F42" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="46" t="n">
+      <c r="G42" s="44" t="n">
         <v>1347.6</v>
       </c>
       <c r="H42" s="44" t="n">
@@ -1914,1110 +1966,1110 @@
       <c r="B43" s="9" t="n"/>
       <c r="C43" s="9" t="n"/>
       <c r="D43" s="10" t="n"/>
-      <c r="E43" s="10" t="n"/>
-      <c r="F43" s="10" t="n"/>
-      <c r="G43" s="41" t="n"/>
-      <c r="H43" s="42" t="n"/>
+      <c r="E43" s="44" t="n"/>
+      <c r="F43" s="44" t="n"/>
+      <c r="G43" s="44" t="n"/>
+      <c r="H43" s="44" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="9" t="n"/>
       <c r="B44" s="9" t="n"/>
       <c r="C44" s="9" t="n"/>
       <c r="D44" s="10" t="n"/>
-      <c r="E44" s="10" t="n"/>
-      <c r="F44" s="10" t="n"/>
-      <c r="G44" s="46" t="n"/>
-      <c r="H44" s="15" t="n"/>
+      <c r="E44" s="44" t="n"/>
+      <c r="F44" s="44" t="n"/>
+      <c r="G44" s="44" t="n"/>
+      <c r="H44" s="44" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="9" t="n"/>
       <c r="B45" s="9" t="n"/>
       <c r="C45" s="9" t="n"/>
       <c r="D45" s="9" t="n"/>
-      <c r="E45" s="9" t="n"/>
-      <c r="F45" s="9" t="n"/>
-      <c r="G45" s="9" t="n"/>
-      <c r="H45" s="9" t="n"/>
+      <c r="E45" s="45" t="n"/>
+      <c r="F45" s="45" t="n"/>
+      <c r="G45" s="45" t="n"/>
+      <c r="H45" s="45" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="9" t="n"/>
       <c r="B46" s="9" t="n"/>
       <c r="C46" s="9" t="n"/>
       <c r="D46" s="9" t="n"/>
-      <c r="E46" s="9" t="n"/>
-      <c r="F46" s="9" t="n"/>
-      <c r="G46" s="9" t="n"/>
-      <c r="H46" s="9" t="n"/>
+      <c r="E46" s="45" t="n"/>
+      <c r="F46" s="45" t="n"/>
+      <c r="G46" s="45" t="n"/>
+      <c r="H46" s="45" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="9" t="n"/>
       <c r="B47" s="9" t="n"/>
       <c r="C47" s="9" t="n"/>
       <c r="D47" s="9" t="n"/>
-      <c r="E47" s="9" t="n"/>
-      <c r="F47" s="9" t="n"/>
-      <c r="G47" s="9" t="n"/>
-      <c r="H47" s="9" t="n"/>
+      <c r="E47" s="45" t="n"/>
+      <c r="F47" s="45" t="n"/>
+      <c r="G47" s="45" t="n"/>
+      <c r="H47" s="45" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="9" t="n"/>
       <c r="B48" s="9" t="n"/>
       <c r="C48" s="9" t="n"/>
       <c r="D48" s="9" t="n"/>
-      <c r="E48" s="9" t="n"/>
-      <c r="F48" s="9" t="n"/>
-      <c r="G48" s="9" t="n"/>
-      <c r="H48" s="9" t="n"/>
+      <c r="E48" s="45" t="n"/>
+      <c r="F48" s="45" t="n"/>
+      <c r="G48" s="45" t="n"/>
+      <c r="H48" s="45" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="9" t="n"/>
       <c r="B49" s="9" t="n"/>
       <c r="C49" s="9" t="n"/>
       <c r="D49" s="9" t="n"/>
-      <c r="E49" s="9" t="n"/>
-      <c r="F49" s="9" t="n"/>
-      <c r="G49" s="9" t="n"/>
-      <c r="H49" s="9" t="n"/>
+      <c r="E49" s="45" t="n"/>
+      <c r="F49" s="45" t="n"/>
+      <c r="G49" s="45" t="n"/>
+      <c r="H49" s="45" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="9" t="n"/>
       <c r="B50" s="9" t="n"/>
       <c r="C50" s="9" t="n"/>
       <c r="D50" s="9" t="n"/>
-      <c r="E50" s="9" t="n"/>
-      <c r="F50" s="9" t="n"/>
-      <c r="G50" s="9" t="n"/>
-      <c r="H50" s="9" t="n"/>
+      <c r="E50" s="45" t="n"/>
+      <c r="F50" s="45" t="n"/>
+      <c r="G50" s="45" t="n"/>
+      <c r="H50" s="45" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="9" t="n"/>
       <c r="B51" s="9" t="n"/>
       <c r="C51" s="9" t="n"/>
       <c r="D51" s="9" t="n"/>
-      <c r="E51" s="9" t="n"/>
-      <c r="F51" s="9" t="n"/>
-      <c r="G51" s="9" t="n"/>
-      <c r="H51" s="9" t="n"/>
+      <c r="E51" s="45" t="n"/>
+      <c r="F51" s="45" t="n"/>
+      <c r="G51" s="45" t="n"/>
+      <c r="H51" s="45" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="9" t="n"/>
       <c r="B52" s="9" t="n"/>
       <c r="C52" s="9" t="n"/>
       <c r="D52" s="9" t="n"/>
-      <c r="E52" s="9" t="n"/>
-      <c r="F52" s="9" t="n"/>
-      <c r="G52" s="9" t="n"/>
-      <c r="H52" s="9" t="n"/>
+      <c r="E52" s="45" t="n"/>
+      <c r="F52" s="45" t="n"/>
+      <c r="G52" s="45" t="n"/>
+      <c r="H52" s="45" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="9" t="n"/>
       <c r="B53" s="9" t="n"/>
       <c r="C53" s="9" t="n"/>
       <c r="D53" s="9" t="n"/>
-      <c r="E53" s="9" t="n"/>
-      <c r="F53" s="9" t="n"/>
-      <c r="G53" s="9" t="n"/>
-      <c r="H53" s="9" t="n"/>
+      <c r="E53" s="45" t="n"/>
+      <c r="F53" s="45" t="n"/>
+      <c r="G53" s="45" t="n"/>
+      <c r="H53" s="45" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="9" t="n"/>
       <c r="B54" s="9" t="n"/>
       <c r="C54" s="9" t="n"/>
       <c r="D54" s="9" t="n"/>
-      <c r="E54" s="9" t="n"/>
-      <c r="F54" s="9" t="n"/>
-      <c r="G54" s="9" t="n"/>
-      <c r="H54" s="9" t="n"/>
+      <c r="E54" s="45" t="n"/>
+      <c r="F54" s="45" t="n"/>
+      <c r="G54" s="45" t="n"/>
+      <c r="H54" s="45" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="9" t="n"/>
       <c r="B55" s="9" t="n"/>
       <c r="C55" s="9" t="n"/>
       <c r="D55" s="9" t="n"/>
-      <c r="E55" s="9" t="n"/>
-      <c r="F55" s="9" t="n"/>
-      <c r="G55" s="9" t="n"/>
-      <c r="H55" s="9" t="n"/>
+      <c r="E55" s="45" t="n"/>
+      <c r="F55" s="45" t="n"/>
+      <c r="G55" s="45" t="n"/>
+      <c r="H55" s="45" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="9" t="n"/>
       <c r="B56" s="9" t="n"/>
       <c r="C56" s="9" t="n"/>
       <c r="D56" s="9" t="n"/>
-      <c r="E56" s="9" t="n"/>
-      <c r="F56" s="9" t="n"/>
-      <c r="G56" s="9" t="n"/>
-      <c r="H56" s="9" t="n"/>
+      <c r="E56" s="45" t="n"/>
+      <c r="F56" s="45" t="n"/>
+      <c r="G56" s="45" t="n"/>
+      <c r="H56" s="45" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="9" t="n"/>
       <c r="B57" s="9" t="n"/>
       <c r="C57" s="9" t="n"/>
       <c r="D57" s="9" t="n"/>
-      <c r="E57" s="9" t="n"/>
-      <c r="F57" s="9" t="n"/>
-      <c r="G57" s="9" t="n"/>
-      <c r="H57" s="9" t="n"/>
+      <c r="E57" s="45" t="n"/>
+      <c r="F57" s="45" t="n"/>
+      <c r="G57" s="45" t="n"/>
+      <c r="H57" s="45" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="9" t="n"/>
       <c r="B58" s="9" t="n"/>
       <c r="C58" s="9" t="n"/>
       <c r="D58" s="9" t="n"/>
-      <c r="E58" s="9" t="n"/>
-      <c r="F58" s="9" t="n"/>
-      <c r="G58" s="9" t="n"/>
-      <c r="H58" s="9" t="n"/>
+      <c r="E58" s="45" t="n"/>
+      <c r="F58" s="45" t="n"/>
+      <c r="G58" s="45" t="n"/>
+      <c r="H58" s="45" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="9" t="n"/>
       <c r="B59" s="9" t="n"/>
       <c r="C59" s="9" t="n"/>
       <c r="D59" s="9" t="n"/>
-      <c r="E59" s="9" t="n"/>
-      <c r="F59" s="9" t="n"/>
-      <c r="G59" s="9" t="n"/>
-      <c r="H59" s="9" t="n"/>
+      <c r="E59" s="45" t="n"/>
+      <c r="F59" s="45" t="n"/>
+      <c r="G59" s="45" t="n"/>
+      <c r="H59" s="45" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="9" t="n"/>
       <c r="B60" s="9" t="n"/>
       <c r="C60" s="9" t="n"/>
       <c r="D60" s="9" t="n"/>
-      <c r="E60" s="9" t="n"/>
-      <c r="F60" s="9" t="n"/>
-      <c r="G60" s="9" t="n"/>
-      <c r="H60" s="9" t="n"/>
+      <c r="E60" s="45" t="n"/>
+      <c r="F60" s="45" t="n"/>
+      <c r="G60" s="45" t="n"/>
+      <c r="H60" s="45" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="9" t="n"/>
       <c r="B61" s="9" t="n"/>
       <c r="C61" s="9" t="n"/>
       <c r="D61" s="9" t="n"/>
-      <c r="E61" s="9" t="n"/>
-      <c r="F61" s="9" t="n"/>
-      <c r="G61" s="9" t="n"/>
-      <c r="H61" s="9" t="n"/>
+      <c r="E61" s="45" t="n"/>
+      <c r="F61" s="45" t="n"/>
+      <c r="G61" s="45" t="n"/>
+      <c r="H61" s="45" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="9" t="n"/>
       <c r="B62" s="9" t="n"/>
       <c r="C62" s="9" t="n"/>
       <c r="D62" s="9" t="n"/>
-      <c r="E62" s="9" t="n"/>
-      <c r="F62" s="9" t="n"/>
-      <c r="G62" s="9" t="n"/>
-      <c r="H62" s="9" t="n"/>
+      <c r="E62" s="45" t="n"/>
+      <c r="F62" s="45" t="n"/>
+      <c r="G62" s="45" t="n"/>
+      <c r="H62" s="45" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="9" t="n"/>
       <c r="B63" s="9" t="n"/>
       <c r="C63" s="9" t="n"/>
       <c r="D63" s="9" t="n"/>
-      <c r="E63" s="9" t="n"/>
-      <c r="F63" s="9" t="n"/>
-      <c r="G63" s="9" t="n"/>
-      <c r="H63" s="9" t="n"/>
+      <c r="E63" s="45" t="n"/>
+      <c r="F63" s="45" t="n"/>
+      <c r="G63" s="45" t="n"/>
+      <c r="H63" s="45" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="9" t="n"/>
       <c r="B64" s="9" t="n"/>
       <c r="C64" s="9" t="n"/>
       <c r="D64" s="9" t="n"/>
-      <c r="E64" s="9" t="n"/>
-      <c r="F64" s="9" t="n"/>
-      <c r="G64" s="9" t="n"/>
-      <c r="H64" s="9" t="n"/>
+      <c r="E64" s="45" t="n"/>
+      <c r="F64" s="45" t="n"/>
+      <c r="G64" s="45" t="n"/>
+      <c r="H64" s="45" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="9" t="n"/>
       <c r="B65" s="9" t="n"/>
       <c r="C65" s="9" t="n"/>
       <c r="D65" s="9" t="n"/>
-      <c r="E65" s="9" t="n"/>
-      <c r="F65" s="9" t="n"/>
-      <c r="G65" s="9" t="n"/>
-      <c r="H65" s="9" t="n"/>
+      <c r="E65" s="45" t="n"/>
+      <c r="F65" s="45" t="n"/>
+      <c r="G65" s="45" t="n"/>
+      <c r="H65" s="45" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="9" t="n"/>
       <c r="B66" s="9" t="n"/>
       <c r="C66" s="9" t="n"/>
       <c r="D66" s="9" t="n"/>
-      <c r="E66" s="9" t="n"/>
-      <c r="F66" s="9" t="n"/>
-      <c r="G66" s="9" t="n"/>
-      <c r="H66" s="9" t="n"/>
+      <c r="E66" s="45" t="n"/>
+      <c r="F66" s="45" t="n"/>
+      <c r="G66" s="45" t="n"/>
+      <c r="H66" s="45" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="9" t="n"/>
       <c r="B67" s="9" t="n"/>
       <c r="C67" s="9" t="n"/>
       <c r="D67" s="9" t="n"/>
-      <c r="E67" s="9" t="n"/>
-      <c r="F67" s="9" t="n"/>
-      <c r="G67" s="9" t="n"/>
-      <c r="H67" s="9" t="n"/>
+      <c r="E67" s="45" t="n"/>
+      <c r="F67" s="45" t="n"/>
+      <c r="G67" s="45" t="n"/>
+      <c r="H67" s="45" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="9" t="n"/>
       <c r="B68" s="9" t="n"/>
       <c r="C68" s="9" t="n"/>
       <c r="D68" s="9" t="n"/>
-      <c r="E68" s="9" t="n"/>
-      <c r="F68" s="9" t="n"/>
-      <c r="G68" s="9" t="n"/>
-      <c r="H68" s="9" t="n"/>
+      <c r="E68" s="45" t="n"/>
+      <c r="F68" s="45" t="n"/>
+      <c r="G68" s="45" t="n"/>
+      <c r="H68" s="45" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="9" t="n"/>
       <c r="B69" s="9" t="n"/>
       <c r="C69" s="9" t="n"/>
       <c r="D69" s="9" t="n"/>
-      <c r="E69" s="9" t="n"/>
-      <c r="F69" s="9" t="n"/>
-      <c r="G69" s="9" t="n"/>
-      <c r="H69" s="9" t="n"/>
+      <c r="E69" s="45" t="n"/>
+      <c r="F69" s="45" t="n"/>
+      <c r="G69" s="45" t="n"/>
+      <c r="H69" s="45" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="9" t="n"/>
       <c r="B70" s="9" t="n"/>
       <c r="C70" s="9" t="n"/>
       <c r="D70" s="9" t="n"/>
-      <c r="E70" s="9" t="n"/>
-      <c r="F70" s="9" t="n"/>
-      <c r="G70" s="9" t="n"/>
-      <c r="H70" s="9" t="n"/>
+      <c r="E70" s="45" t="n"/>
+      <c r="F70" s="45" t="n"/>
+      <c r="G70" s="45" t="n"/>
+      <c r="H70" s="45" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="9" t="n"/>
       <c r="B71" s="9" t="n"/>
       <c r="C71" s="9" t="n"/>
       <c r="D71" s="9" t="n"/>
-      <c r="E71" s="9" t="n"/>
-      <c r="F71" s="9" t="n"/>
-      <c r="G71" s="9" t="n"/>
-      <c r="H71" s="9" t="n"/>
+      <c r="E71" s="45" t="n"/>
+      <c r="F71" s="45" t="n"/>
+      <c r="G71" s="45" t="n"/>
+      <c r="H71" s="45" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="9" t="n"/>
       <c r="B72" s="9" t="n"/>
       <c r="C72" s="9" t="n"/>
       <c r="D72" s="9" t="n"/>
-      <c r="E72" s="9" t="n"/>
-      <c r="F72" s="9" t="n"/>
-      <c r="G72" s="9" t="n"/>
-      <c r="H72" s="9" t="n"/>
+      <c r="E72" s="45" t="n"/>
+      <c r="F72" s="45" t="n"/>
+      <c r="G72" s="45" t="n"/>
+      <c r="H72" s="45" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="9" t="n"/>
       <c r="B73" s="9" t="n"/>
       <c r="C73" s="9" t="n"/>
       <c r="D73" s="9" t="n"/>
-      <c r="E73" s="9" t="n"/>
-      <c r="F73" s="9" t="n"/>
-      <c r="G73" s="9" t="n"/>
-      <c r="H73" s="9" t="n"/>
+      <c r="E73" s="45" t="n"/>
+      <c r="F73" s="45" t="n"/>
+      <c r="G73" s="45" t="n"/>
+      <c r="H73" s="45" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="9" t="n"/>
       <c r="B74" s="9" t="n"/>
       <c r="C74" s="9" t="n"/>
       <c r="D74" s="9" t="n"/>
-      <c r="E74" s="9" t="n"/>
-      <c r="F74" s="9" t="n"/>
-      <c r="G74" s="9" t="n"/>
-      <c r="H74" s="9" t="n"/>
+      <c r="E74" s="45" t="n"/>
+      <c r="F74" s="45" t="n"/>
+      <c r="G74" s="45" t="n"/>
+      <c r="H74" s="45" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="9" t="n"/>
       <c r="B75" s="9" t="n"/>
       <c r="C75" s="9" t="n"/>
       <c r="D75" s="9" t="n"/>
-      <c r="E75" s="9" t="n"/>
-      <c r="F75" s="9" t="n"/>
-      <c r="G75" s="9" t="n"/>
-      <c r="H75" s="9" t="n"/>
+      <c r="E75" s="45" t="n"/>
+      <c r="F75" s="45" t="n"/>
+      <c r="G75" s="45" t="n"/>
+      <c r="H75" s="45" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="9" t="n"/>
       <c r="B76" s="9" t="n"/>
       <c r="C76" s="9" t="n"/>
       <c r="D76" s="9" t="n"/>
-      <c r="E76" s="9" t="n"/>
-      <c r="F76" s="9" t="n"/>
-      <c r="G76" s="9" t="n"/>
-      <c r="H76" s="9" t="n"/>
+      <c r="E76" s="45" t="n"/>
+      <c r="F76" s="45" t="n"/>
+      <c r="G76" s="45" t="n"/>
+      <c r="H76" s="45" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="9" t="n"/>
       <c r="B77" s="9" t="n"/>
       <c r="C77" s="9" t="n"/>
       <c r="D77" s="9" t="n"/>
-      <c r="E77" s="9" t="n"/>
-      <c r="F77" s="9" t="n"/>
-      <c r="G77" s="9" t="n"/>
-      <c r="H77" s="9" t="n"/>
+      <c r="E77" s="45" t="n"/>
+      <c r="F77" s="45" t="n"/>
+      <c r="G77" s="45" t="n"/>
+      <c r="H77" s="45" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="9" t="n"/>
       <c r="B78" s="9" t="n"/>
       <c r="C78" s="9" t="n"/>
       <c r="D78" s="9" t="n"/>
-      <c r="E78" s="9" t="n"/>
-      <c r="F78" s="9" t="n"/>
-      <c r="G78" s="9" t="n"/>
-      <c r="H78" s="9" t="n"/>
+      <c r="E78" s="45" t="n"/>
+      <c r="F78" s="45" t="n"/>
+      <c r="G78" s="45" t="n"/>
+      <c r="H78" s="45" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="9" t="n"/>
       <c r="B79" s="9" t="n"/>
       <c r="C79" s="9" t="n"/>
       <c r="D79" s="9" t="n"/>
-      <c r="E79" s="9" t="n"/>
-      <c r="F79" s="9" t="n"/>
-      <c r="G79" s="9" t="n"/>
-      <c r="H79" s="9" t="n"/>
+      <c r="E79" s="45" t="n"/>
+      <c r="F79" s="45" t="n"/>
+      <c r="G79" s="45" t="n"/>
+      <c r="H79" s="45" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="9" t="n"/>
       <c r="B80" s="9" t="n"/>
       <c r="C80" s="9" t="n"/>
       <c r="D80" s="9" t="n"/>
-      <c r="E80" s="9" t="n"/>
-      <c r="F80" s="9" t="n"/>
-      <c r="G80" s="9" t="n"/>
-      <c r="H80" s="9" t="n"/>
+      <c r="E80" s="45" t="n"/>
+      <c r="F80" s="45" t="n"/>
+      <c r="G80" s="45" t="n"/>
+      <c r="H80" s="45" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="9" t="n"/>
       <c r="B81" s="9" t="n"/>
       <c r="C81" s="9" t="n"/>
       <c r="D81" s="9" t="n"/>
-      <c r="E81" s="9" t="n"/>
-      <c r="F81" s="9" t="n"/>
-      <c r="G81" s="9" t="n"/>
-      <c r="H81" s="9" t="n"/>
+      <c r="E81" s="45" t="n"/>
+      <c r="F81" s="45" t="n"/>
+      <c r="G81" s="45" t="n"/>
+      <c r="H81" s="45" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="9" t="n"/>
       <c r="B82" s="9" t="n"/>
       <c r="C82" s="9" t="n"/>
       <c r="D82" s="9" t="n"/>
-      <c r="E82" s="9" t="n"/>
-      <c r="F82" s="9" t="n"/>
-      <c r="G82" s="9" t="n"/>
-      <c r="H82" s="9" t="n"/>
+      <c r="E82" s="45" t="n"/>
+      <c r="F82" s="45" t="n"/>
+      <c r="G82" s="45" t="n"/>
+      <c r="H82" s="45" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="9" t="n"/>
       <c r="B83" s="9" t="n"/>
       <c r="C83" s="9" t="n"/>
       <c r="D83" s="9" t="n"/>
-      <c r="E83" s="9" t="n"/>
-      <c r="F83" s="9" t="n"/>
-      <c r="G83" s="9" t="n"/>
-      <c r="H83" s="9" t="n"/>
+      <c r="E83" s="45" t="n"/>
+      <c r="F83" s="45" t="n"/>
+      <c r="G83" s="45" t="n"/>
+      <c r="H83" s="45" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="9" t="n"/>
       <c r="B84" s="9" t="n"/>
       <c r="C84" s="9" t="n"/>
       <c r="D84" s="9" t="n"/>
-      <c r="E84" s="9" t="n"/>
-      <c r="F84" s="9" t="n"/>
-      <c r="G84" s="9" t="n"/>
-      <c r="H84" s="9" t="n"/>
+      <c r="E84" s="45" t="n"/>
+      <c r="F84" s="45" t="n"/>
+      <c r="G84" s="45" t="n"/>
+      <c r="H84" s="45" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="9" t="n"/>
       <c r="B85" s="9" t="n"/>
       <c r="C85" s="9" t="n"/>
       <c r="D85" s="9" t="n"/>
-      <c r="E85" s="9" t="n"/>
-      <c r="F85" s="9" t="n"/>
-      <c r="G85" s="9" t="n"/>
-      <c r="H85" s="9" t="n"/>
+      <c r="E85" s="45" t="n"/>
+      <c r="F85" s="45" t="n"/>
+      <c r="G85" s="45" t="n"/>
+      <c r="H85" s="45" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="9" t="n"/>
       <c r="B86" s="9" t="n"/>
       <c r="C86" s="9" t="n"/>
       <c r="D86" s="9" t="n"/>
-      <c r="E86" s="9" t="n"/>
-      <c r="F86" s="9" t="n"/>
-      <c r="G86" s="9" t="n"/>
-      <c r="H86" s="9" t="n"/>
+      <c r="E86" s="45" t="n"/>
+      <c r="F86" s="45" t="n"/>
+      <c r="G86" s="45" t="n"/>
+      <c r="H86" s="45" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="9" t="n"/>
       <c r="B87" s="9" t="n"/>
       <c r="C87" s="9" t="n"/>
       <c r="D87" s="9" t="n"/>
-      <c r="E87" s="9" t="n"/>
-      <c r="F87" s="9" t="n"/>
-      <c r="G87" s="9" t="n"/>
-      <c r="H87" s="9" t="n"/>
+      <c r="E87" s="45" t="n"/>
+      <c r="F87" s="45" t="n"/>
+      <c r="G87" s="45" t="n"/>
+      <c r="H87" s="45" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="9" t="n"/>
       <c r="B88" s="9" t="n"/>
       <c r="C88" s="9" t="n"/>
       <c r="D88" s="9" t="n"/>
-      <c r="E88" s="9" t="n"/>
-      <c r="F88" s="9" t="n"/>
-      <c r="G88" s="9" t="n"/>
-      <c r="H88" s="9" t="n"/>
+      <c r="E88" s="45" t="n"/>
+      <c r="F88" s="45" t="n"/>
+      <c r="G88" s="45" t="n"/>
+      <c r="H88" s="45" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="9" t="n"/>
       <c r="B89" s="9" t="n"/>
       <c r="C89" s="9" t="n"/>
       <c r="D89" s="9" t="n"/>
-      <c r="E89" s="9" t="n"/>
-      <c r="F89" s="9" t="n"/>
-      <c r="G89" s="9" t="n"/>
-      <c r="H89" s="9" t="n"/>
+      <c r="E89" s="45" t="n"/>
+      <c r="F89" s="45" t="n"/>
+      <c r="G89" s="45" t="n"/>
+      <c r="H89" s="45" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="9" t="n"/>
       <c r="B90" s="9" t="n"/>
       <c r="C90" s="9" t="n"/>
       <c r="D90" s="9" t="n"/>
-      <c r="E90" s="9" t="n"/>
-      <c r="F90" s="9" t="n"/>
-      <c r="G90" s="9" t="n"/>
-      <c r="H90" s="9" t="n"/>
+      <c r="E90" s="45" t="n"/>
+      <c r="F90" s="45" t="n"/>
+      <c r="G90" s="45" t="n"/>
+      <c r="H90" s="45" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="9" t="n"/>
       <c r="B91" s="9" t="n"/>
       <c r="C91" s="9" t="n"/>
       <c r="D91" s="9" t="n"/>
-      <c r="E91" s="9" t="n"/>
-      <c r="F91" s="9" t="n"/>
-      <c r="G91" s="9" t="n"/>
-      <c r="H91" s="9" t="n"/>
+      <c r="E91" s="45" t="n"/>
+      <c r="F91" s="45" t="n"/>
+      <c r="G91" s="45" t="n"/>
+      <c r="H91" s="45" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="9" t="n"/>
       <c r="B92" s="9" t="n"/>
       <c r="C92" s="9" t="n"/>
       <c r="D92" s="9" t="n"/>
-      <c r="E92" s="9" t="n"/>
-      <c r="F92" s="9" t="n"/>
-      <c r="G92" s="9" t="n"/>
-      <c r="H92" s="9" t="n"/>
+      <c r="E92" s="45" t="n"/>
+      <c r="F92" s="45" t="n"/>
+      <c r="G92" s="45" t="n"/>
+      <c r="H92" s="45" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="9" t="n"/>
       <c r="B93" s="9" t="n"/>
       <c r="C93" s="9" t="n"/>
       <c r="D93" s="9" t="n"/>
-      <c r="E93" s="9" t="n"/>
-      <c r="F93" s="9" t="n"/>
-      <c r="G93" s="9" t="n"/>
-      <c r="H93" s="9" t="n"/>
+      <c r="E93" s="45" t="n"/>
+      <c r="F93" s="45" t="n"/>
+      <c r="G93" s="45" t="n"/>
+      <c r="H93" s="45" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="9" t="n"/>
       <c r="B94" s="9" t="n"/>
       <c r="C94" s="9" t="n"/>
       <c r="D94" s="9" t="n"/>
-      <c r="E94" s="9" t="n"/>
-      <c r="F94" s="9" t="n"/>
-      <c r="G94" s="9" t="n"/>
-      <c r="H94" s="9" t="n"/>
+      <c r="E94" s="45" t="n"/>
+      <c r="F94" s="45" t="n"/>
+      <c r="G94" s="45" t="n"/>
+      <c r="H94" s="45" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="9" t="n"/>
       <c r="B95" s="9" t="n"/>
       <c r="C95" s="9" t="n"/>
       <c r="D95" s="9" t="n"/>
-      <c r="E95" s="9" t="n"/>
-      <c r="F95" s="9" t="n"/>
-      <c r="G95" s="9" t="n"/>
-      <c r="H95" s="9" t="n"/>
+      <c r="E95" s="45" t="n"/>
+      <c r="F95" s="45" t="n"/>
+      <c r="G95" s="45" t="n"/>
+      <c r="H95" s="45" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="9" t="n"/>
       <c r="B96" s="9" t="n"/>
       <c r="C96" s="9" t="n"/>
       <c r="D96" s="9" t="n"/>
-      <c r="E96" s="9" t="n"/>
-      <c r="F96" s="9" t="n"/>
-      <c r="G96" s="9" t="n"/>
-      <c r="H96" s="9" t="n"/>
+      <c r="E96" s="45" t="n"/>
+      <c r="F96" s="45" t="n"/>
+      <c r="G96" s="45" t="n"/>
+      <c r="H96" s="45" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="9" t="n"/>
       <c r="B97" s="9" t="n"/>
       <c r="C97" s="9" t="n"/>
       <c r="D97" s="9" t="n"/>
-      <c r="E97" s="9" t="n"/>
-      <c r="F97" s="9" t="n"/>
-      <c r="G97" s="9" t="n"/>
-      <c r="H97" s="9" t="n"/>
+      <c r="E97" s="45" t="n"/>
+      <c r="F97" s="45" t="n"/>
+      <c r="G97" s="45" t="n"/>
+      <c r="H97" s="45" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="9" t="n"/>
       <c r="B98" s="9" t="n"/>
       <c r="C98" s="9" t="n"/>
       <c r="D98" s="9" t="n"/>
-      <c r="E98" s="9" t="n"/>
-      <c r="F98" s="9" t="n"/>
-      <c r="G98" s="9" t="n"/>
-      <c r="H98" s="9" t="n"/>
+      <c r="E98" s="45" t="n"/>
+      <c r="F98" s="45" t="n"/>
+      <c r="G98" s="45" t="n"/>
+      <c r="H98" s="45" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="9" t="n"/>
       <c r="B99" s="9" t="n"/>
       <c r="C99" s="9" t="n"/>
       <c r="D99" s="9" t="n"/>
-      <c r="E99" s="9" t="n"/>
-      <c r="F99" s="9" t="n"/>
-      <c r="G99" s="9" t="n"/>
-      <c r="H99" s="9" t="n"/>
+      <c r="E99" s="45" t="n"/>
+      <c r="F99" s="45" t="n"/>
+      <c r="G99" s="45" t="n"/>
+      <c r="H99" s="45" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="9" t="n"/>
       <c r="B100" s="9" t="n"/>
       <c r="C100" s="9" t="n"/>
       <c r="D100" s="9" t="n"/>
-      <c r="E100" s="9" t="n"/>
-      <c r="F100" s="9" t="n"/>
-      <c r="G100" s="9" t="n"/>
-      <c r="H100" s="9" t="n"/>
+      <c r="E100" s="45" t="n"/>
+      <c r="F100" s="45" t="n"/>
+      <c r="G100" s="45" t="n"/>
+      <c r="H100" s="45" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="9" t="n"/>
       <c r="B101" s="9" t="n"/>
       <c r="C101" s="9" t="n"/>
       <c r="D101" s="9" t="n"/>
-      <c r="E101" s="9" t="n"/>
-      <c r="F101" s="9" t="n"/>
-      <c r="G101" s="9" t="n"/>
-      <c r="H101" s="9" t="n"/>
+      <c r="E101" s="45" t="n"/>
+      <c r="F101" s="45" t="n"/>
+      <c r="G101" s="45" t="n"/>
+      <c r="H101" s="45" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="9" t="n"/>
       <c r="B102" s="9" t="n"/>
       <c r="C102" s="9" t="n"/>
       <c r="D102" s="9" t="n"/>
-      <c r="E102" s="9" t="n"/>
-      <c r="F102" s="9" t="n"/>
-      <c r="G102" s="9" t="n"/>
-      <c r="H102" s="9" t="n"/>
+      <c r="E102" s="45" t="n"/>
+      <c r="F102" s="45" t="n"/>
+      <c r="G102" s="45" t="n"/>
+      <c r="H102" s="45" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="9" t="n"/>
       <c r="B103" s="9" t="n"/>
       <c r="C103" s="9" t="n"/>
       <c r="D103" s="9" t="n"/>
-      <c r="E103" s="9" t="n"/>
-      <c r="F103" s="9" t="n"/>
-      <c r="G103" s="9" t="n"/>
-      <c r="H103" s="9" t="n"/>
+      <c r="E103" s="45" t="n"/>
+      <c r="F103" s="45" t="n"/>
+      <c r="G103" s="45" t="n"/>
+      <c r="H103" s="45" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="9" t="n"/>
       <c r="B104" s="9" t="n"/>
       <c r="C104" s="9" t="n"/>
       <c r="D104" s="9" t="n"/>
-      <c r="E104" s="9" t="n"/>
-      <c r="F104" s="9" t="n"/>
-      <c r="G104" s="9" t="n"/>
-      <c r="H104" s="9" t="n"/>
+      <c r="E104" s="45" t="n"/>
+      <c r="F104" s="45" t="n"/>
+      <c r="G104" s="45" t="n"/>
+      <c r="H104" s="45" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="9" t="n"/>
       <c r="B105" s="9" t="n"/>
       <c r="C105" s="9" t="n"/>
       <c r="D105" s="9" t="n"/>
-      <c r="E105" s="9" t="n"/>
-      <c r="F105" s="9" t="n"/>
-      <c r="G105" s="9" t="n"/>
-      <c r="H105" s="9" t="n"/>
+      <c r="E105" s="45" t="n"/>
+      <c r="F105" s="45" t="n"/>
+      <c r="G105" s="45" t="n"/>
+      <c r="H105" s="45" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="9" t="n"/>
       <c r="B106" s="9" t="n"/>
       <c r="C106" s="9" t="n"/>
       <c r="D106" s="9" t="n"/>
-      <c r="E106" s="9" t="n"/>
-      <c r="F106" s="9" t="n"/>
-      <c r="G106" s="9" t="n"/>
-      <c r="H106" s="9" t="n"/>
+      <c r="E106" s="45" t="n"/>
+      <c r="F106" s="45" t="n"/>
+      <c r="G106" s="45" t="n"/>
+      <c r="H106" s="45" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="9" t="n"/>
       <c r="B107" s="9" t="n"/>
       <c r="C107" s="9" t="n"/>
       <c r="D107" s="9" t="n"/>
-      <c r="E107" s="9" t="n"/>
-      <c r="F107" s="9" t="n"/>
-      <c r="G107" s="9" t="n"/>
-      <c r="H107" s="9" t="n"/>
+      <c r="E107" s="45" t="n"/>
+      <c r="F107" s="45" t="n"/>
+      <c r="G107" s="45" t="n"/>
+      <c r="H107" s="45" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="9" t="n"/>
       <c r="B108" s="9" t="n"/>
       <c r="C108" s="9" t="n"/>
       <c r="D108" s="9" t="n"/>
-      <c r="E108" s="9" t="n"/>
-      <c r="F108" s="9" t="n"/>
-      <c r="G108" s="9" t="n"/>
-      <c r="H108" s="9" t="n"/>
+      <c r="E108" s="45" t="n"/>
+      <c r="F108" s="45" t="n"/>
+      <c r="G108" s="45" t="n"/>
+      <c r="H108" s="45" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="9" t="n"/>
       <c r="B109" s="9" t="n"/>
       <c r="C109" s="9" t="n"/>
       <c r="D109" s="9" t="n"/>
-      <c r="E109" s="9" t="n"/>
-      <c r="F109" s="9" t="n"/>
-      <c r="G109" s="9" t="n"/>
-      <c r="H109" s="9" t="n"/>
+      <c r="E109" s="45" t="n"/>
+      <c r="F109" s="45" t="n"/>
+      <c r="G109" s="45" t="n"/>
+      <c r="H109" s="45" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="9" t="n"/>
       <c r="B110" s="9" t="n"/>
       <c r="C110" s="9" t="n"/>
       <c r="D110" s="9" t="n"/>
-      <c r="E110" s="9" t="n"/>
-      <c r="F110" s="9" t="n"/>
-      <c r="G110" s="9" t="n"/>
-      <c r="H110" s="9" t="n"/>
+      <c r="E110" s="45" t="n"/>
+      <c r="F110" s="45" t="n"/>
+      <c r="G110" s="45" t="n"/>
+      <c r="H110" s="45" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="9" t="n"/>
       <c r="B111" s="9" t="n"/>
       <c r="C111" s="9" t="n"/>
       <c r="D111" s="9" t="n"/>
-      <c r="E111" s="9" t="n"/>
-      <c r="F111" s="9" t="n"/>
-      <c r="G111" s="9" t="n"/>
-      <c r="H111" s="9" t="n"/>
+      <c r="E111" s="45" t="n"/>
+      <c r="F111" s="45" t="n"/>
+      <c r="G111" s="45" t="n"/>
+      <c r="H111" s="45" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="9" t="n"/>
       <c r="B112" s="9" t="n"/>
       <c r="C112" s="9" t="n"/>
       <c r="D112" s="9" t="n"/>
-      <c r="E112" s="9" t="n"/>
-      <c r="F112" s="9" t="n"/>
-      <c r="G112" s="9" t="n"/>
-      <c r="H112" s="9" t="n"/>
+      <c r="E112" s="45" t="n"/>
+      <c r="F112" s="45" t="n"/>
+      <c r="G112" s="45" t="n"/>
+      <c r="H112" s="45" t="n"/>
     </row>
     <row r="113">
       <c r="A113" s="9" t="n"/>
       <c r="B113" s="9" t="n"/>
       <c r="C113" s="9" t="n"/>
       <c r="D113" s="9" t="n"/>
-      <c r="E113" s="9" t="n"/>
-      <c r="F113" s="9" t="n"/>
-      <c r="G113" s="9" t="n"/>
-      <c r="H113" s="9" t="n"/>
+      <c r="E113" s="45" t="n"/>
+      <c r="F113" s="45" t="n"/>
+      <c r="G113" s="45" t="n"/>
+      <c r="H113" s="45" t="n"/>
     </row>
     <row r="114">
       <c r="A114" s="9" t="n"/>
       <c r="B114" s="9" t="n"/>
       <c r="C114" s="9" t="n"/>
       <c r="D114" s="9" t="n"/>
-      <c r="E114" s="9" t="n"/>
-      <c r="F114" s="9" t="n"/>
-      <c r="G114" s="9" t="n"/>
-      <c r="H114" s="9" t="n"/>
+      <c r="E114" s="45" t="n"/>
+      <c r="F114" s="45" t="n"/>
+      <c r="G114" s="45" t="n"/>
+      <c r="H114" s="45" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="9" t="n"/>
       <c r="B115" s="9" t="n"/>
       <c r="C115" s="9" t="n"/>
       <c r="D115" s="9" t="n"/>
-      <c r="E115" s="9" t="n"/>
-      <c r="F115" s="9" t="n"/>
-      <c r="G115" s="9" t="n"/>
-      <c r="H115" s="9" t="n"/>
+      <c r="E115" s="45" t="n"/>
+      <c r="F115" s="45" t="n"/>
+      <c r="G115" s="45" t="n"/>
+      <c r="H115" s="45" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="9" t="n"/>
       <c r="B116" s="9" t="n"/>
       <c r="C116" s="9" t="n"/>
       <c r="D116" s="9" t="n"/>
-      <c r="E116" s="9" t="n"/>
-      <c r="F116" s="9" t="n"/>
-      <c r="G116" s="9" t="n"/>
-      <c r="H116" s="9" t="n"/>
+      <c r="E116" s="45" t="n"/>
+      <c r="F116" s="45" t="n"/>
+      <c r="G116" s="45" t="n"/>
+      <c r="H116" s="45" t="n"/>
     </row>
     <row r="117">
       <c r="A117" s="9" t="n"/>
       <c r="B117" s="9" t="n"/>
       <c r="C117" s="9" t="n"/>
       <c r="D117" s="9" t="n"/>
-      <c r="E117" s="9" t="n"/>
-      <c r="F117" s="9" t="n"/>
-      <c r="G117" s="9" t="n"/>
-      <c r="H117" s="9" t="n"/>
+      <c r="E117" s="45" t="n"/>
+      <c r="F117" s="45" t="n"/>
+      <c r="G117" s="45" t="n"/>
+      <c r="H117" s="45" t="n"/>
     </row>
     <row r="118">
       <c r="A118" s="9" t="n"/>
       <c r="B118" s="9" t="n"/>
       <c r="C118" s="9" t="n"/>
       <c r="D118" s="9" t="n"/>
-      <c r="E118" s="9" t="n"/>
-      <c r="F118" s="9" t="n"/>
-      <c r="G118" s="9" t="n"/>
-      <c r="H118" s="9" t="n"/>
+      <c r="E118" s="45" t="n"/>
+      <c r="F118" s="45" t="n"/>
+      <c r="G118" s="45" t="n"/>
+      <c r="H118" s="45" t="n"/>
     </row>
     <row r="119">
       <c r="A119" s="9" t="n"/>
       <c r="B119" s="9" t="n"/>
       <c r="C119" s="9" t="n"/>
       <c r="D119" s="9" t="n"/>
-      <c r="E119" s="9" t="n"/>
-      <c r="F119" s="9" t="n"/>
-      <c r="G119" s="9" t="n"/>
-      <c r="H119" s="9" t="n"/>
+      <c r="E119" s="45" t="n"/>
+      <c r="F119" s="45" t="n"/>
+      <c r="G119" s="45" t="n"/>
+      <c r="H119" s="45" t="n"/>
     </row>
     <row r="120">
       <c r="A120" s="9" t="n"/>
       <c r="B120" s="9" t="n"/>
       <c r="C120" s="9" t="n"/>
       <c r="D120" s="9" t="n"/>
-      <c r="E120" s="9" t="n"/>
-      <c r="F120" s="9" t="n"/>
-      <c r="G120" s="9" t="n"/>
-      <c r="H120" s="9" t="n"/>
+      <c r="E120" s="45" t="n"/>
+      <c r="F120" s="45" t="n"/>
+      <c r="G120" s="45" t="n"/>
+      <c r="H120" s="45" t="n"/>
     </row>
     <row r="121">
       <c r="A121" s="9" t="n"/>
       <c r="B121" s="9" t="n"/>
       <c r="C121" s="9" t="n"/>
       <c r="D121" s="9" t="n"/>
-      <c r="E121" s="9" t="n"/>
-      <c r="F121" s="9" t="n"/>
-      <c r="G121" s="9" t="n"/>
-      <c r="H121" s="9" t="n"/>
+      <c r="E121" s="45" t="n"/>
+      <c r="F121" s="45" t="n"/>
+      <c r="G121" s="45" t="n"/>
+      <c r="H121" s="45" t="n"/>
     </row>
     <row r="122">
       <c r="A122" s="9" t="n"/>
       <c r="B122" s="9" t="n"/>
       <c r="C122" s="9" t="n"/>
       <c r="D122" s="9" t="n"/>
-      <c r="E122" s="9" t="n"/>
-      <c r="F122" s="9" t="n"/>
-      <c r="G122" s="9" t="n"/>
-      <c r="H122" s="9" t="n"/>
+      <c r="E122" s="45" t="n"/>
+      <c r="F122" s="45" t="n"/>
+      <c r="G122" s="45" t="n"/>
+      <c r="H122" s="45" t="n"/>
     </row>
     <row r="123">
       <c r="A123" s="9" t="n"/>
       <c r="B123" s="9" t="n"/>
       <c r="C123" s="9" t="n"/>
       <c r="D123" s="9" t="n"/>
-      <c r="E123" s="9" t="n"/>
-      <c r="F123" s="9" t="n"/>
-      <c r="G123" s="9" t="n"/>
-      <c r="H123" s="9" t="n"/>
+      <c r="E123" s="45" t="n"/>
+      <c r="F123" s="45" t="n"/>
+      <c r="G123" s="45" t="n"/>
+      <c r="H123" s="45" t="n"/>
     </row>
     <row r="124">
       <c r="A124" s="9" t="n"/>
       <c r="B124" s="9" t="n"/>
       <c r="C124" s="9" t="n"/>
       <c r="D124" s="9" t="n"/>
-      <c r="E124" s="9" t="n"/>
-      <c r="F124" s="9" t="n"/>
-      <c r="G124" s="9" t="n"/>
-      <c r="H124" s="9" t="n"/>
+      <c r="E124" s="45" t="n"/>
+      <c r="F124" s="45" t="n"/>
+      <c r="G124" s="45" t="n"/>
+      <c r="H124" s="45" t="n"/>
     </row>
     <row r="125">
       <c r="A125" s="9" t="n"/>
       <c r="B125" s="9" t="n"/>
       <c r="C125" s="9" t="n"/>
       <c r="D125" s="9" t="n"/>
-      <c r="E125" s="9" t="n"/>
-      <c r="F125" s="9" t="n"/>
-      <c r="G125" s="9" t="n"/>
-      <c r="H125" s="9" t="n"/>
+      <c r="E125" s="45" t="n"/>
+      <c r="F125" s="45" t="n"/>
+      <c r="G125" s="45" t="n"/>
+      <c r="H125" s="45" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="9" t="n"/>
       <c r="B126" s="9" t="n"/>
       <c r="C126" s="9" t="n"/>
       <c r="D126" s="9" t="n"/>
-      <c r="E126" s="9" t="n"/>
-      <c r="F126" s="9" t="n"/>
-      <c r="G126" s="9" t="n"/>
-      <c r="H126" s="9" t="n"/>
+      <c r="E126" s="45" t="n"/>
+      <c r="F126" s="45" t="n"/>
+      <c r="G126" s="45" t="n"/>
+      <c r="H126" s="45" t="n"/>
     </row>
     <row r="127">
       <c r="A127" s="9" t="n"/>
       <c r="B127" s="9" t="n"/>
       <c r="C127" s="9" t="n"/>
       <c r="D127" s="9" t="n"/>
-      <c r="E127" s="9" t="n"/>
-      <c r="F127" s="9" t="n"/>
-      <c r="G127" s="9" t="n"/>
-      <c r="H127" s="9" t="n"/>
+      <c r="E127" s="45" t="n"/>
+      <c r="F127" s="45" t="n"/>
+      <c r="G127" s="45" t="n"/>
+      <c r="H127" s="45" t="n"/>
     </row>
     <row r="128">
       <c r="A128" s="9" t="n"/>
       <c r="B128" s="9" t="n"/>
       <c r="C128" s="9" t="n"/>
       <c r="D128" s="9" t="n"/>
-      <c r="E128" s="9" t="n"/>
-      <c r="F128" s="9" t="n"/>
-      <c r="G128" s="9" t="n"/>
-      <c r="H128" s="9" t="n"/>
+      <c r="E128" s="45" t="n"/>
+      <c r="F128" s="45" t="n"/>
+      <c r="G128" s="45" t="n"/>
+      <c r="H128" s="45" t="n"/>
     </row>
     <row r="129">
       <c r="A129" s="9" t="n"/>
       <c r="B129" s="9" t="n"/>
       <c r="C129" s="9" t="n"/>
       <c r="D129" s="9" t="n"/>
-      <c r="E129" s="9" t="n"/>
-      <c r="F129" s="9" t="n"/>
-      <c r="G129" s="9" t="n"/>
-      <c r="H129" s="9" t="n"/>
+      <c r="E129" s="45" t="n"/>
+      <c r="F129" s="45" t="n"/>
+      <c r="G129" s="45" t="n"/>
+      <c r="H129" s="45" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="9" t="n"/>
       <c r="B130" s="9" t="n"/>
       <c r="C130" s="9" t="n"/>
       <c r="D130" s="9" t="n"/>
-      <c r="E130" s="9" t="n"/>
-      <c r="F130" s="9" t="n"/>
-      <c r="G130" s="9" t="n"/>
-      <c r="H130" s="9" t="n"/>
+      <c r="E130" s="45" t="n"/>
+      <c r="F130" s="45" t="n"/>
+      <c r="G130" s="45" t="n"/>
+      <c r="H130" s="45" t="n"/>
     </row>
     <row r="131">
       <c r="A131" s="9" t="n"/>
       <c r="B131" s="9" t="n"/>
       <c r="C131" s="9" t="n"/>
       <c r="D131" s="9" t="n"/>
-      <c r="E131" s="9" t="n"/>
-      <c r="F131" s="9" t="n"/>
-      <c r="G131" s="9" t="n"/>
-      <c r="H131" s="9" t="n"/>
+      <c r="E131" s="45" t="n"/>
+      <c r="F131" s="45" t="n"/>
+      <c r="G131" s="45" t="n"/>
+      <c r="H131" s="45" t="n"/>
     </row>
     <row r="132">
       <c r="A132" s="9" t="n"/>
       <c r="B132" s="9" t="n"/>
       <c r="C132" s="9" t="n"/>
       <c r="D132" s="9" t="n"/>
-      <c r="E132" s="9" t="n"/>
-      <c r="F132" s="9" t="n"/>
-      <c r="G132" s="9" t="n"/>
-      <c r="H132" s="9" t="n"/>
+      <c r="E132" s="45" t="n"/>
+      <c r="F132" s="45" t="n"/>
+      <c r="G132" s="45" t="n"/>
+      <c r="H132" s="45" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="9" t="n"/>
       <c r="B133" s="9" t="n"/>
       <c r="C133" s="9" t="n"/>
       <c r="D133" s="9" t="n"/>
-      <c r="E133" s="9" t="n"/>
-      <c r="F133" s="9" t="n"/>
-      <c r="G133" s="9" t="n"/>
-      <c r="H133" s="9" t="n"/>
+      <c r="E133" s="45" t="n"/>
+      <c r="F133" s="45" t="n"/>
+      <c r="G133" s="45" t="n"/>
+      <c r="H133" s="45" t="n"/>
     </row>
     <row r="134">
       <c r="A134" s="9" t="n"/>
       <c r="B134" s="9" t="n"/>
       <c r="C134" s="9" t="n"/>
       <c r="D134" s="9" t="n"/>
-      <c r="E134" s="9" t="n"/>
-      <c r="F134" s="9" t="n"/>
-      <c r="G134" s="9" t="n"/>
-      <c r="H134" s="9" t="n"/>
+      <c r="E134" s="45" t="n"/>
+      <c r="F134" s="45" t="n"/>
+      <c r="G134" s="45" t="n"/>
+      <c r="H134" s="45" t="n"/>
     </row>
     <row r="135">
       <c r="A135" s="9" t="n"/>
       <c r="B135" s="9" t="n"/>
       <c r="C135" s="9" t="n"/>
       <c r="D135" s="9" t="n"/>
-      <c r="E135" s="9" t="n"/>
-      <c r="F135" s="9" t="n"/>
-      <c r="G135" s="9" t="n"/>
-      <c r="H135" s="9" t="n"/>
+      <c r="E135" s="45" t="n"/>
+      <c r="F135" s="45" t="n"/>
+      <c r="G135" s="45" t="n"/>
+      <c r="H135" s="45" t="n"/>
     </row>
     <row r="136">
       <c r="A136" s="9" t="n"/>
       <c r="B136" s="9" t="n"/>
       <c r="C136" s="9" t="n"/>
       <c r="D136" s="9" t="n"/>
-      <c r="E136" s="9" t="n"/>
-      <c r="F136" s="9" t="n"/>
-      <c r="G136" s="9" t="n"/>
-      <c r="H136" s="9" t="n"/>
+      <c r="E136" s="45" t="n"/>
+      <c r="F136" s="45" t="n"/>
+      <c r="G136" s="45" t="n"/>
+      <c r="H136" s="45" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="9" t="n"/>
       <c r="B137" s="9" t="n"/>
       <c r="C137" s="9" t="n"/>
       <c r="D137" s="9" t="n"/>
-      <c r="E137" s="9" t="n"/>
-      <c r="F137" s="9" t="n"/>
-      <c r="G137" s="9" t="n"/>
-      <c r="H137" s="9" t="n"/>
+      <c r="E137" s="45" t="n"/>
+      <c r="F137" s="45" t="n"/>
+      <c r="G137" s="45" t="n"/>
+      <c r="H137" s="45" t="n"/>
     </row>
     <row r="138">
       <c r="A138" s="9" t="n"/>
       <c r="B138" s="9" t="n"/>
       <c r="C138" s="9" t="n"/>
       <c r="D138" s="9" t="n"/>
-      <c r="E138" s="9" t="n"/>
-      <c r="F138" s="9" t="n"/>
-      <c r="G138" s="9" t="n"/>
-      <c r="H138" s="9" t="n"/>
+      <c r="E138" s="45" t="n"/>
+      <c r="F138" s="45" t="n"/>
+      <c r="G138" s="45" t="n"/>
+      <c r="H138" s="45" t="n"/>
     </row>
     <row r="139">
       <c r="A139" s="9" t="n"/>
       <c r="B139" s="9" t="n"/>
       <c r="C139" s="9" t="n"/>
       <c r="D139" s="9" t="n"/>
-      <c r="E139" s="9" t="n"/>
-      <c r="F139" s="9" t="n"/>
-      <c r="G139" s="9" t="n"/>
-      <c r="H139" s="9" t="n"/>
+      <c r="E139" s="45" t="n"/>
+      <c r="F139" s="45" t="n"/>
+      <c r="G139" s="45" t="n"/>
+      <c r="H139" s="45" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="9" t="n"/>
       <c r="B140" s="9" t="n"/>
       <c r="C140" s="9" t="n"/>
       <c r="D140" s="9" t="n"/>
-      <c r="E140" s="9" t="n"/>
-      <c r="F140" s="9" t="n"/>
-      <c r="G140" s="9" t="n"/>
-      <c r="H140" s="9" t="n"/>
+      <c r="E140" s="45" t="n"/>
+      <c r="F140" s="45" t="n"/>
+      <c r="G140" s="45" t="n"/>
+      <c r="H140" s="45" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="9" t="n"/>
       <c r="B141" s="9" t="n"/>
       <c r="C141" s="9" t="n"/>
       <c r="D141" s="9" t="n"/>
-      <c r="E141" s="9" t="n"/>
-      <c r="F141" s="9" t="n"/>
-      <c r="G141" s="9" t="n"/>
-      <c r="H141" s="9" t="n"/>
+      <c r="E141" s="45" t="n"/>
+      <c r="F141" s="45" t="n"/>
+      <c r="G141" s="45" t="n"/>
+      <c r="H141" s="45" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="9" t="n"/>
       <c r="B142" s="9" t="n"/>
       <c r="C142" s="9" t="n"/>
       <c r="D142" s="9" t="n"/>
-      <c r="E142" s="9" t="n"/>
-      <c r="F142" s="9" t="n"/>
-      <c r="G142" s="9" t="n"/>
-      <c r="H142" s="9" t="n"/>
+      <c r="E142" s="45" t="n"/>
+      <c r="F142" s="45" t="n"/>
+      <c r="G142" s="45" t="n"/>
+      <c r="H142" s="45" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="9" t="n"/>
       <c r="B143" s="9" t="n"/>
       <c r="C143" s="9" t="n"/>
       <c r="D143" s="9" t="n"/>
-      <c r="E143" s="9" t="n"/>
-      <c r="F143" s="9" t="n"/>
-      <c r="G143" s="9" t="n"/>
-      <c r="H143" s="9" t="n"/>
+      <c r="E143" s="45" t="n"/>
+      <c r="F143" s="45" t="n"/>
+      <c r="G143" s="45" t="n"/>
+      <c r="H143" s="45" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="9" t="n"/>
       <c r="B144" s="9" t="n"/>
       <c r="C144" s="9" t="n"/>
       <c r="D144" s="9" t="n"/>
-      <c r="E144" s="9" t="n"/>
-      <c r="F144" s="9" t="n"/>
-      <c r="G144" s="9" t="n"/>
-      <c r="H144" s="9" t="n"/>
+      <c r="E144" s="45" t="n"/>
+      <c r="F144" s="45" t="n"/>
+      <c r="G144" s="45" t="n"/>
+      <c r="H144" s="45" t="n"/>
     </row>
     <row r="145">
       <c r="A145" s="9" t="n"/>
       <c r="B145" s="9" t="n"/>
       <c r="C145" s="9" t="n"/>
       <c r="D145" s="9" t="n"/>
-      <c r="E145" s="9" t="n"/>
-      <c r="F145" s="9" t="n"/>
-      <c r="G145" s="9" t="n"/>
-      <c r="H145" s="9" t="n"/>
+      <c r="E145" s="45" t="n"/>
+      <c r="F145" s="45" t="n"/>
+      <c r="G145" s="45" t="n"/>
+      <c r="H145" s="45" t="n"/>
     </row>
     <row r="146">
       <c r="A146" s="9" t="n"/>
       <c r="B146" s="9" t="n"/>
       <c r="C146" s="9" t="n"/>
       <c r="D146" s="9" t="n"/>
-      <c r="E146" s="9" t="n"/>
-      <c r="F146" s="9" t="n"/>
-      <c r="G146" s="9" t="n"/>
-      <c r="H146" s="9" t="n"/>
+      <c r="E146" s="45" t="n"/>
+      <c r="F146" s="45" t="n"/>
+      <c r="G146" s="45" t="n"/>
+      <c r="H146" s="45" t="n"/>
     </row>
     <row r="147">
       <c r="A147" s="9" t="n"/>
       <c r="B147" s="9" t="n"/>
       <c r="C147" s="9" t="n"/>
       <c r="D147" s="9" t="n"/>
-      <c r="E147" s="9" t="n"/>
-      <c r="F147" s="9" t="n"/>
-      <c r="G147" s="9" t="n"/>
-      <c r="H147" s="9" t="n"/>
+      <c r="E147" s="45" t="n"/>
+      <c r="F147" s="45" t="n"/>
+      <c r="G147" s="45" t="n"/>
+      <c r="H147" s="45" t="n"/>
     </row>
     <row r="148">
       <c r="A148" s="9" t="n"/>
       <c r="B148" s="9" t="n"/>
       <c r="C148" s="9" t="n"/>
       <c r="D148" s="9" t="n"/>
-      <c r="E148" s="9" t="n"/>
-      <c r="F148" s="9" t="n"/>
-      <c r="G148" s="9" t="n"/>
-      <c r="H148" s="9" t="n"/>
+      <c r="E148" s="45" t="n"/>
+      <c r="F148" s="45" t="n"/>
+      <c r="G148" s="45" t="n"/>
+      <c r="H148" s="45" t="n"/>
     </row>
     <row r="149">
       <c r="A149" s="9" t="n"/>
       <c r="B149" s="9" t="n"/>
       <c r="C149" s="9" t="n"/>
       <c r="D149" s="9" t="n"/>
-      <c r="E149" s="9" t="n"/>
-      <c r="F149" s="9" t="n"/>
-      <c r="G149" s="9" t="n"/>
-      <c r="H149" s="9" t="n"/>
+      <c r="E149" s="45" t="n"/>
+      <c r="F149" s="45" t="n"/>
+      <c r="G149" s="45" t="n"/>
+      <c r="H149" s="45" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="9" t="n"/>
       <c r="B150" s="9" t="n"/>
       <c r="C150" s="9" t="n"/>
       <c r="D150" s="9" t="n"/>
-      <c r="E150" s="9" t="n"/>
-      <c r="F150" s="9" t="n"/>
-      <c r="G150" s="9" t="n"/>
-      <c r="H150" s="9" t="n"/>
+      <c r="E150" s="45" t="n"/>
+      <c r="F150" s="45" t="n"/>
+      <c r="G150" s="45" t="n"/>
+      <c r="H150" s="45" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="9" t="n"/>
       <c r="B151" s="9" t="n"/>
       <c r="C151" s="9" t="n"/>
       <c r="D151" s="9" t="n"/>
-      <c r="E151" s="9" t="n"/>
-      <c r="F151" s="9" t="n"/>
-      <c r="G151" s="9" t="n"/>
-      <c r="H151" s="9" t="n"/>
+      <c r="E151" s="45" t="n"/>
+      <c r="F151" s="45" t="n"/>
+      <c r="G151" s="45" t="n"/>
+      <c r="H151" s="45" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="9" t="n"/>
       <c r="B152" s="9" t="n"/>
       <c r="C152" s="9" t="n"/>
       <c r="D152" s="9" t="n"/>
-      <c r="E152" s="9" t="n"/>
-      <c r="F152" s="9" t="n"/>
-      <c r="G152" s="9" t="n"/>
-      <c r="H152" s="9" t="n"/>
+      <c r="E152" s="45" t="n"/>
+      <c r="F152" s="45" t="n"/>
+      <c r="G152" s="45" t="n"/>
+      <c r="H152" s="45" t="n"/>
     </row>
     <row r="153">
       <c r="A153" s="9" t="n"/>
       <c r="B153" s="9" t="n"/>
       <c r="C153" s="9" t="n"/>
       <c r="D153" s="9" t="n"/>
-      <c r="E153" s="9" t="n"/>
-      <c r="F153" s="9" t="n"/>
-      <c r="G153" s="9" t="n"/>
-      <c r="H153" s="9" t="n"/>
+      <c r="E153" s="45" t="n"/>
+      <c r="F153" s="45" t="n"/>
+      <c r="G153" s="45" t="n"/>
+      <c r="H153" s="45" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3026,12 +3078,12 @@
   </mergeCells>
   <pageMargins left="0.5299999713897705" right="0.5299999713897705" top="0.5299999713897705" bottom="0.6899999976158142" header="0" footer="0"/>
   <pageSetup orientation="landscape" paperSize="9" scale="0" fitToHeight="0" fitToWidth="0" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -3057,32 +3109,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>PLANILHA ORÇAMENTÁRIA</t>
         </is>
       </c>
-      <c r="B1" s="32" t="n"/>
-      <c r="C1" s="32" t="n"/>
-      <c r="D1" s="32" t="n"/>
-      <c r="E1" s="32" t="n"/>
-      <c r="F1" s="32" t="n"/>
-      <c r="G1" s="32" t="n"/>
-      <c r="H1" s="33" t="n"/>
+      <c r="B1" s="36" t="n"/>
+      <c r="C1" s="36" t="n"/>
+      <c r="D1" s="36" t="n"/>
+      <c r="E1" s="36" t="n"/>
+      <c r="F1" s="36" t="n"/>
+      <c r="G1" s="36" t="n"/>
+      <c r="H1" s="37" t="n"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="34" t="n"/>
-      <c r="H2" s="35" t="n"/>
+      <c r="A2" s="38" t="n"/>
+      <c r="H2" s="39" t="n"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="36" t="n"/>
-      <c r="B3" s="37" t="n"/>
-      <c r="C3" s="37" t="n"/>
-      <c r="D3" s="37" t="n"/>
-      <c r="E3" s="37" t="n"/>
-      <c r="F3" s="37" t="n"/>
-      <c r="G3" s="37" t="n"/>
-      <c r="H3" s="38" t="n"/>
+      <c r="A3" s="40" t="n"/>
+      <c r="B3" s="41" t="n"/>
+      <c r="C3" s="41" t="n"/>
+      <c r="D3" s="41" t="n"/>
+      <c r="E3" s="41" t="n"/>
+      <c r="F3" s="41" t="n"/>
+      <c r="G3" s="41" t="n"/>
+      <c r="H3" s="42" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
@@ -3140,7 +3192,7 @@
       <c r="E8" s="8" t="n"/>
       <c r="F8" s="8" t="n"/>
       <c r="G8" s="8" t="n"/>
-      <c r="H8" s="39" t="n"/>
+      <c r="H8" s="43" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
@@ -3150,7 +3202,7 @@
       <c r="E9" s="8" t="n"/>
       <c r="F9" s="8" t="n"/>
       <c r="G9" s="8" t="n"/>
-      <c r="H9" s="39" t="n"/>
+      <c r="H9" s="43" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="21" t="n"/>
@@ -3205,7 +3257,7 @@
       <c r="E12" s="10" t="n"/>
       <c r="F12" s="10" t="n"/>
       <c r="G12" s="10" t="n"/>
-      <c r="H12" s="40" t="n"/>
+      <c r="H12" s="46" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="20" t="n"/>
@@ -3224,8 +3276,8 @@
       <c r="D14" s="10" t="n"/>
       <c r="E14" s="10" t="n"/>
       <c r="F14" s="10" t="n"/>
-      <c r="G14" s="41" t="n"/>
-      <c r="H14" s="42" t="n"/>
+      <c r="G14" s="47" t="n"/>
+      <c r="H14" s="48" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="n"/>
@@ -3234,7 +3286,7 @@
       <c r="D15" s="10" t="n"/>
       <c r="E15" s="10" t="n"/>
       <c r="F15" s="10" t="n"/>
-      <c r="G15" s="43" t="n"/>
+      <c r="G15" s="49" t="n"/>
       <c r="H15" s="15" t="n"/>
     </row>
     <row r="16">
@@ -3245,7 +3297,7 @@
       <c r="E16" s="10" t="n"/>
       <c r="F16" s="10" t="n"/>
       <c r="G16" s="10" t="n"/>
-      <c r="H16" s="44" t="n"/>
+      <c r="H16" s="50" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="9" t="n"/>
@@ -3254,7 +3306,7 @@
       <c r="D17" s="10" t="n"/>
       <c r="E17" s="10" t="n"/>
       <c r="F17" s="10" t="n"/>
-      <c r="G17" s="45" t="n"/>
+      <c r="G17" s="51" t="n"/>
       <c r="H17" s="15" t="n"/>
     </row>
     <row r="18">
@@ -3264,7 +3316,7 @@
       <c r="D18" s="10" t="n"/>
       <c r="E18" s="10" t="n"/>
       <c r="F18" s="10" t="n"/>
-      <c r="G18" s="41" t="n"/>
+      <c r="G18" s="47" t="n"/>
       <c r="H18" s="15" t="n"/>
     </row>
     <row r="19">
@@ -3274,7 +3326,7 @@
       <c r="D19" s="10" t="n"/>
       <c r="E19" s="10" t="n"/>
       <c r="F19" s="10" t="n"/>
-      <c r="G19" s="43" t="n"/>
+      <c r="G19" s="49" t="n"/>
       <c r="H19" s="15" t="n"/>
     </row>
     <row r="20">
@@ -3284,7 +3336,7 @@
       <c r="D20" s="10" t="n"/>
       <c r="E20" s="10" t="n"/>
       <c r="F20" s="10" t="n"/>
-      <c r="G20" s="43" t="n"/>
+      <c r="G20" s="49" t="n"/>
       <c r="H20" s="15" t="n"/>
     </row>
     <row r="21">
@@ -3293,8 +3345,8 @@
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="10" t="n"/>
       <c r="E21" s="10" t="n"/>
-      <c r="F21" s="46" t="n"/>
-      <c r="G21" s="46" t="n"/>
+      <c r="F21" s="52" t="n"/>
+      <c r="G21" s="52" t="n"/>
       <c r="H21" s="15" t="n"/>
     </row>
     <row r="22">
@@ -3305,7 +3357,7 @@
       <c r="E22" s="10" t="n"/>
       <c r="F22" s="10" t="n"/>
       <c r="G22" s="10" t="n"/>
-      <c r="H22" s="44" t="n"/>
+      <c r="H22" s="50" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="9" t="n"/>
@@ -3315,7 +3367,7 @@
       <c r="E23" s="10" t="n"/>
       <c r="F23" s="10" t="n"/>
       <c r="G23" s="10" t="n"/>
-      <c r="H23" s="44" t="n"/>
+      <c r="H23" s="50" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="9" t="n"/>
@@ -3324,18 +3376,18 @@
       <c r="D24" s="10" t="n"/>
       <c r="E24" s="10" t="n"/>
       <c r="F24" s="10" t="n"/>
-      <c r="G24" s="41" t="n"/>
-      <c r="H24" s="44" t="n"/>
+      <c r="G24" s="47" t="n"/>
+      <c r="H24" s="50" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
       <c r="D25" s="10" t="n"/>
-      <c r="E25" s="45" t="n"/>
-      <c r="F25" s="45" t="n"/>
-      <c r="G25" s="45" t="n"/>
-      <c r="H25" s="42" t="n"/>
+      <c r="E25" s="51" t="n"/>
+      <c r="F25" s="51" t="n"/>
+      <c r="G25" s="51" t="n"/>
+      <c r="H25" s="48" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="9" t="n"/>
@@ -3344,7 +3396,7 @@
       <c r="D26" s="10" t="n"/>
       <c r="E26" s="10" t="n"/>
       <c r="F26" s="10" t="n"/>
-      <c r="G26" s="41" t="n"/>
+      <c r="G26" s="47" t="n"/>
       <c r="H26" s="15" t="n"/>
     </row>
     <row r="27">
@@ -3354,7 +3406,7 @@
       <c r="D27" s="10" t="n"/>
       <c r="E27" s="10" t="n"/>
       <c r="F27" s="10" t="n"/>
-      <c r="G27" s="41" t="n"/>
+      <c r="G27" s="47" t="n"/>
       <c r="H27" s="15" t="n"/>
     </row>
     <row r="28">
@@ -3364,7 +3416,7 @@
       <c r="D28" s="10" t="n"/>
       <c r="E28" s="10" t="n"/>
       <c r="F28" s="10" t="n"/>
-      <c r="G28" s="41" t="n"/>
+      <c r="G28" s="47" t="n"/>
       <c r="H28" s="15" t="n"/>
     </row>
     <row r="29">
@@ -3373,8 +3425,8 @@
       <c r="C29" s="9" t="n"/>
       <c r="D29" s="10" t="n"/>
       <c r="E29" s="10" t="n"/>
-      <c r="F29" s="41" t="n"/>
-      <c r="G29" s="41" t="n"/>
+      <c r="F29" s="47" t="n"/>
+      <c r="G29" s="47" t="n"/>
       <c r="H29" s="15" t="n"/>
     </row>
     <row r="30">
@@ -3383,9 +3435,9 @@
       <c r="C30" s="9" t="n"/>
       <c r="D30" s="10" t="n"/>
       <c r="E30" s="10" t="n"/>
-      <c r="F30" s="41" t="n"/>
-      <c r="G30" s="41" t="n"/>
-      <c r="H30" s="44" t="n"/>
+      <c r="F30" s="47" t="n"/>
+      <c r="G30" s="47" t="n"/>
+      <c r="H30" s="50" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="9" t="n"/>
@@ -3394,7 +3446,7 @@
       <c r="D31" s="10" t="n"/>
       <c r="E31" s="10" t="n"/>
       <c r="F31" s="10" t="n"/>
-      <c r="G31" s="41" t="n"/>
+      <c r="G31" s="47" t="n"/>
       <c r="H31" s="15" t="n"/>
     </row>
     <row r="32">
@@ -3404,7 +3456,7 @@
       <c r="D32" s="10" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
-      <c r="G32" s="41" t="n"/>
+      <c r="G32" s="47" t="n"/>
       <c r="H32" s="15" t="n"/>
     </row>
     <row r="33">
@@ -3415,7 +3467,7 @@
       <c r="E33" s="10" t="n"/>
       <c r="F33" s="10" t="n"/>
       <c r="G33" s="10" t="n"/>
-      <c r="H33" s="44" t="n"/>
+      <c r="H33" s="50" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="9" t="n"/>
@@ -3424,17 +3476,17 @@
       <c r="D34" s="10" t="n"/>
       <c r="E34" s="10" t="n"/>
       <c r="F34" s="10" t="n"/>
-      <c r="G34" s="43" t="n"/>
-      <c r="H34" s="42" t="n"/>
+      <c r="G34" s="49" t="n"/>
+      <c r="H34" s="48" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="9" t="n"/>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="9" t="n"/>
       <c r="D35" s="10" t="n"/>
-      <c r="E35" s="43" t="n"/>
+      <c r="E35" s="49" t="n"/>
       <c r="F35" s="10" t="n"/>
-      <c r="G35" s="43" t="n"/>
+      <c r="G35" s="49" t="n"/>
       <c r="H35" s="15" t="n"/>
     </row>
     <row r="36">
@@ -3442,9 +3494,9 @@
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
       <c r="D36" s="10" t="n"/>
-      <c r="E36" s="46" t="n"/>
+      <c r="E36" s="52" t="n"/>
       <c r="F36" s="10" t="n"/>
-      <c r="G36" s="46" t="n"/>
+      <c r="G36" s="52" t="n"/>
       <c r="H36" s="15" t="n"/>
     </row>
     <row r="37">
@@ -3454,7 +3506,7 @@
       <c r="D37" s="10" t="n"/>
       <c r="E37" s="10" t="n"/>
       <c r="F37" s="10" t="n"/>
-      <c r="G37" s="46" t="n"/>
+      <c r="G37" s="52" t="n"/>
       <c r="H37" s="15" t="n"/>
     </row>
     <row r="38">
@@ -3464,27 +3516,27 @@
       <c r="D38" s="10" t="n"/>
       <c r="E38" s="10" t="n"/>
       <c r="F38" s="10" t="n"/>
-      <c r="G38" s="43" t="n"/>
-      <c r="H38" s="42" t="n"/>
+      <c r="G38" s="49" t="n"/>
+      <c r="H38" s="48" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="9" t="n"/>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="9" t="n"/>
       <c r="D39" s="10" t="n"/>
-      <c r="E39" s="43" t="n"/>
-      <c r="F39" s="43" t="n"/>
-      <c r="G39" s="43" t="n"/>
-      <c r="H39" s="42" t="n"/>
+      <c r="E39" s="49" t="n"/>
+      <c r="F39" s="49" t="n"/>
+      <c r="G39" s="49" t="n"/>
+      <c r="H39" s="48" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="9" t="n"/>
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="9" t="n"/>
       <c r="D40" s="10" t="n"/>
-      <c r="E40" s="46" t="n"/>
+      <c r="E40" s="52" t="n"/>
       <c r="F40" s="10" t="n"/>
-      <c r="G40" s="46" t="n"/>
+      <c r="G40" s="52" t="n"/>
       <c r="H40" s="15" t="n"/>
     </row>
     <row r="41">
@@ -3495,7 +3547,7 @@
       <c r="E41" s="10" t="n"/>
       <c r="F41" s="10" t="n"/>
       <c r="G41" s="10" t="n"/>
-      <c r="H41" s="44" t="n"/>
+      <c r="H41" s="50" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="9" t="n"/>
@@ -3504,8 +3556,8 @@
       <c r="D42" s="10" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
-      <c r="G42" s="46" t="n"/>
-      <c r="H42" s="44" t="n"/>
+      <c r="G42" s="52" t="n"/>
+      <c r="H42" s="50" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="9" t="n"/>
@@ -3514,8 +3566,8 @@
       <c r="D43" s="10" t="n"/>
       <c r="E43" s="10" t="n"/>
       <c r="F43" s="10" t="n"/>
-      <c r="G43" s="41" t="n"/>
-      <c r="H43" s="42" t="n"/>
+      <c r="G43" s="47" t="n"/>
+      <c r="H43" s="48" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="9" t="n"/>
@@ -3524,7 +3576,7 @@
       <c r="D44" s="10" t="n"/>
       <c r="E44" s="10" t="n"/>
       <c r="F44" s="10" t="n"/>
-      <c r="G44" s="46" t="n"/>
+      <c r="G44" s="52" t="n"/>
       <c r="H44" s="15" t="n"/>
     </row>
     <row r="45">
@@ -4624,12 +4676,12 @@
   </mergeCells>
   <pageMargins left="0.5299999713897705" right="0.5299999713897705" top="0.5299999713897705" bottom="0.6899999976158142" header="0" footer="0"/>
   <pageSetup orientation="landscape" paperSize="9" scale="0" fitToHeight="0" fitToWidth="0" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4655,32 +4707,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>PLANILHA ORÇAMENTÁRIA</t>
         </is>
       </c>
-      <c r="B1" s="32" t="n"/>
-      <c r="C1" s="32" t="n"/>
-      <c r="D1" s="32" t="n"/>
-      <c r="E1" s="32" t="n"/>
-      <c r="F1" s="32" t="n"/>
-      <c r="G1" s="32" t="n"/>
-      <c r="H1" s="33" t="n"/>
+      <c r="B1" s="36" t="n"/>
+      <c r="C1" s="36" t="n"/>
+      <c r="D1" s="36" t="n"/>
+      <c r="E1" s="36" t="n"/>
+      <c r="F1" s="36" t="n"/>
+      <c r="G1" s="36" t="n"/>
+      <c r="H1" s="37" t="n"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="34" t="n"/>
-      <c r="H2" s="35" t="n"/>
+      <c r="A2" s="38" t="n"/>
+      <c r="H2" s="39" t="n"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="36" t="n"/>
-      <c r="B3" s="37" t="n"/>
-      <c r="C3" s="37" t="n"/>
-      <c r="D3" s="37" t="n"/>
-      <c r="E3" s="37" t="n"/>
-      <c r="F3" s="37" t="n"/>
-      <c r="G3" s="37" t="n"/>
-      <c r="H3" s="38" t="n"/>
+      <c r="A3" s="40" t="n"/>
+      <c r="B3" s="41" t="n"/>
+      <c r="C3" s="41" t="n"/>
+      <c r="D3" s="41" t="n"/>
+      <c r="E3" s="41" t="n"/>
+      <c r="F3" s="41" t="n"/>
+      <c r="G3" s="41" t="n"/>
+      <c r="H3" s="42" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
@@ -4738,7 +4790,7 @@
       <c r="E8" s="8" t="n"/>
       <c r="F8" s="8" t="n"/>
       <c r="G8" s="8" t="n"/>
-      <c r="H8" s="39" t="n"/>
+      <c r="H8" s="43" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
@@ -4748,7 +4800,7 @@
       <c r="E9" s="8" t="n"/>
       <c r="F9" s="8" t="n"/>
       <c r="G9" s="8" t="n"/>
-      <c r="H9" s="39" t="n"/>
+      <c r="H9" s="43" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="21" t="n"/>
@@ -4803,7 +4855,7 @@
       <c r="E12" s="10" t="n"/>
       <c r="F12" s="10" t="n"/>
       <c r="G12" s="10" t="n"/>
-      <c r="H12" s="40" t="n"/>
+      <c r="H12" s="46" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="20" t="n"/>
@@ -4822,8 +4874,8 @@
       <c r="D14" s="10" t="n"/>
       <c r="E14" s="10" t="n"/>
       <c r="F14" s="10" t="n"/>
-      <c r="G14" s="41" t="n"/>
-      <c r="H14" s="42" t="n"/>
+      <c r="G14" s="47" t="n"/>
+      <c r="H14" s="48" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="n"/>
@@ -4832,7 +4884,7 @@
       <c r="D15" s="10" t="n"/>
       <c r="E15" s="10" t="n"/>
       <c r="F15" s="10" t="n"/>
-      <c r="G15" s="43" t="n"/>
+      <c r="G15" s="49" t="n"/>
       <c r="H15" s="15" t="n"/>
     </row>
     <row r="16">
@@ -4843,7 +4895,7 @@
       <c r="E16" s="10" t="n"/>
       <c r="F16" s="10" t="n"/>
       <c r="G16" s="10" t="n"/>
-      <c r="H16" s="44" t="n"/>
+      <c r="H16" s="50" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="9" t="n"/>
@@ -4852,7 +4904,7 @@
       <c r="D17" s="10" t="n"/>
       <c r="E17" s="10" t="n"/>
       <c r="F17" s="10" t="n"/>
-      <c r="G17" s="45" t="n"/>
+      <c r="G17" s="51" t="n"/>
       <c r="H17" s="15" t="n"/>
     </row>
     <row r="18">
@@ -4862,7 +4914,7 @@
       <c r="D18" s="10" t="n"/>
       <c r="E18" s="10" t="n"/>
       <c r="F18" s="10" t="n"/>
-      <c r="G18" s="41" t="n"/>
+      <c r="G18" s="47" t="n"/>
       <c r="H18" s="15" t="n"/>
     </row>
     <row r="19">
@@ -4872,7 +4924,7 @@
       <c r="D19" s="10" t="n"/>
       <c r="E19" s="10" t="n"/>
       <c r="F19" s="10" t="n"/>
-      <c r="G19" s="43" t="n"/>
+      <c r="G19" s="49" t="n"/>
       <c r="H19" s="15" t="n"/>
     </row>
     <row r="20">
@@ -4882,7 +4934,7 @@
       <c r="D20" s="10" t="n"/>
       <c r="E20" s="10" t="n"/>
       <c r="F20" s="10" t="n"/>
-      <c r="G20" s="43" t="n"/>
+      <c r="G20" s="49" t="n"/>
       <c r="H20" s="15" t="n"/>
     </row>
     <row r="21">
@@ -4891,8 +4943,8 @@
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="10" t="n"/>
       <c r="E21" s="10" t="n"/>
-      <c r="F21" s="46" t="n"/>
-      <c r="G21" s="46" t="n"/>
+      <c r="F21" s="52" t="n"/>
+      <c r="G21" s="52" t="n"/>
       <c r="H21" s="15" t="n"/>
     </row>
     <row r="22">
@@ -4903,7 +4955,7 @@
       <c r="E22" s="10" t="n"/>
       <c r="F22" s="10" t="n"/>
       <c r="G22" s="10" t="n"/>
-      <c r="H22" s="44" t="n"/>
+      <c r="H22" s="50" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="9" t="n"/>
@@ -4913,7 +4965,7 @@
       <c r="E23" s="10" t="n"/>
       <c r="F23" s="10" t="n"/>
       <c r="G23" s="10" t="n"/>
-      <c r="H23" s="44" t="n"/>
+      <c r="H23" s="50" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="9" t="n"/>
@@ -4922,18 +4974,18 @@
       <c r="D24" s="10" t="n"/>
       <c r="E24" s="10" t="n"/>
       <c r="F24" s="10" t="n"/>
-      <c r="G24" s="41" t="n"/>
-      <c r="H24" s="44" t="n"/>
+      <c r="G24" s="47" t="n"/>
+      <c r="H24" s="50" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
       <c r="D25" s="10" t="n"/>
-      <c r="E25" s="45" t="n"/>
-      <c r="F25" s="45" t="n"/>
-      <c r="G25" s="45" t="n"/>
-      <c r="H25" s="42" t="n"/>
+      <c r="E25" s="51" t="n"/>
+      <c r="F25" s="51" t="n"/>
+      <c r="G25" s="51" t="n"/>
+      <c r="H25" s="48" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="9" t="n"/>
@@ -4942,7 +4994,7 @@
       <c r="D26" s="10" t="n"/>
       <c r="E26" s="10" t="n"/>
       <c r="F26" s="10" t="n"/>
-      <c r="G26" s="41" t="n"/>
+      <c r="G26" s="47" t="n"/>
       <c r="H26" s="15" t="n"/>
     </row>
     <row r="27">
@@ -4952,7 +5004,7 @@
       <c r="D27" s="10" t="n"/>
       <c r="E27" s="10" t="n"/>
       <c r="F27" s="10" t="n"/>
-      <c r="G27" s="41" t="n"/>
+      <c r="G27" s="47" t="n"/>
       <c r="H27" s="15" t="n"/>
     </row>
     <row r="28">
@@ -4962,7 +5014,7 @@
       <c r="D28" s="10" t="n"/>
       <c r="E28" s="10" t="n"/>
       <c r="F28" s="10" t="n"/>
-      <c r="G28" s="41" t="n"/>
+      <c r="G28" s="47" t="n"/>
       <c r="H28" s="15" t="n"/>
     </row>
     <row r="29">
@@ -4971,8 +5023,8 @@
       <c r="C29" s="9" t="n"/>
       <c r="D29" s="10" t="n"/>
       <c r="E29" s="10" t="n"/>
-      <c r="F29" s="41" t="n"/>
-      <c r="G29" s="41" t="n"/>
+      <c r="F29" s="47" t="n"/>
+      <c r="G29" s="47" t="n"/>
       <c r="H29" s="15" t="n"/>
     </row>
     <row r="30">
@@ -4981,9 +5033,9 @@
       <c r="C30" s="9" t="n"/>
       <c r="D30" s="10" t="n"/>
       <c r="E30" s="10" t="n"/>
-      <c r="F30" s="41" t="n"/>
-      <c r="G30" s="41" t="n"/>
-      <c r="H30" s="44" t="n"/>
+      <c r="F30" s="47" t="n"/>
+      <c r="G30" s="47" t="n"/>
+      <c r="H30" s="50" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="9" t="n"/>
@@ -4992,7 +5044,7 @@
       <c r="D31" s="10" t="n"/>
       <c r="E31" s="10" t="n"/>
       <c r="F31" s="10" t="n"/>
-      <c r="G31" s="41" t="n"/>
+      <c r="G31" s="47" t="n"/>
       <c r="H31" s="15" t="n"/>
     </row>
     <row r="32">
@@ -5002,7 +5054,7 @@
       <c r="D32" s="10" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
-      <c r="G32" s="41" t="n"/>
+      <c r="G32" s="47" t="n"/>
       <c r="H32" s="15" t="n"/>
     </row>
     <row r="33">
@@ -5013,7 +5065,7 @@
       <c r="E33" s="10" t="n"/>
       <c r="F33" s="10" t="n"/>
       <c r="G33" s="10" t="n"/>
-      <c r="H33" s="44" t="n"/>
+      <c r="H33" s="50" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="9" t="n"/>
@@ -5022,17 +5074,17 @@
       <c r="D34" s="10" t="n"/>
       <c r="E34" s="10" t="n"/>
       <c r="F34" s="10" t="n"/>
-      <c r="G34" s="43" t="n"/>
-      <c r="H34" s="42" t="n"/>
+      <c r="G34" s="49" t="n"/>
+      <c r="H34" s="48" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="9" t="n"/>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="9" t="n"/>
       <c r="D35" s="10" t="n"/>
-      <c r="E35" s="43" t="n"/>
+      <c r="E35" s="49" t="n"/>
       <c r="F35" s="10" t="n"/>
-      <c r="G35" s="43" t="n"/>
+      <c r="G35" s="49" t="n"/>
       <c r="H35" s="15" t="n"/>
     </row>
     <row r="36">
@@ -5040,9 +5092,9 @@
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
       <c r="D36" s="10" t="n"/>
-      <c r="E36" s="46" t="n"/>
+      <c r="E36" s="52" t="n"/>
       <c r="F36" s="10" t="n"/>
-      <c r="G36" s="46" t="n"/>
+      <c r="G36" s="52" t="n"/>
       <c r="H36" s="15" t="n"/>
     </row>
     <row r="37">
@@ -5052,7 +5104,7 @@
       <c r="D37" s="10" t="n"/>
       <c r="E37" s="10" t="n"/>
       <c r="F37" s="10" t="n"/>
-      <c r="G37" s="46" t="n"/>
+      <c r="G37" s="52" t="n"/>
       <c r="H37" s="15" t="n"/>
     </row>
     <row r="38">
@@ -5062,27 +5114,27 @@
       <c r="D38" s="10" t="n"/>
       <c r="E38" s="10" t="n"/>
       <c r="F38" s="10" t="n"/>
-      <c r="G38" s="43" t="n"/>
-      <c r="H38" s="42" t="n"/>
+      <c r="G38" s="49" t="n"/>
+      <c r="H38" s="48" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="9" t="n"/>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="9" t="n"/>
       <c r="D39" s="10" t="n"/>
-      <c r="E39" s="43" t="n"/>
-      <c r="F39" s="43" t="n"/>
-      <c r="G39" s="43" t="n"/>
-      <c r="H39" s="42" t="n"/>
+      <c r="E39" s="49" t="n"/>
+      <c r="F39" s="49" t="n"/>
+      <c r="G39" s="49" t="n"/>
+      <c r="H39" s="48" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="9" t="n"/>
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="9" t="n"/>
       <c r="D40" s="10" t="n"/>
-      <c r="E40" s="46" t="n"/>
+      <c r="E40" s="52" t="n"/>
       <c r="F40" s="10" t="n"/>
-      <c r="G40" s="46" t="n"/>
+      <c r="G40" s="52" t="n"/>
       <c r="H40" s="15" t="n"/>
     </row>
     <row r="41">
@@ -5093,7 +5145,7 @@
       <c r="E41" s="10" t="n"/>
       <c r="F41" s="10" t="n"/>
       <c r="G41" s="10" t="n"/>
-      <c r="H41" s="44" t="n"/>
+      <c r="H41" s="50" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="9" t="n"/>
@@ -5102,8 +5154,8 @@
       <c r="D42" s="10" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
-      <c r="G42" s="46" t="n"/>
-      <c r="H42" s="44" t="n"/>
+      <c r="G42" s="52" t="n"/>
+      <c r="H42" s="50" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="9" t="n"/>
@@ -5112,8 +5164,8 @@
       <c r="D43" s="10" t="n"/>
       <c r="E43" s="10" t="n"/>
       <c r="F43" s="10" t="n"/>
-      <c r="G43" s="41" t="n"/>
-      <c r="H43" s="42" t="n"/>
+      <c r="G43" s="47" t="n"/>
+      <c r="H43" s="48" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="9" t="n"/>
@@ -5122,7 +5174,7 @@
       <c r="D44" s="10" t="n"/>
       <c r="E44" s="10" t="n"/>
       <c r="F44" s="10" t="n"/>
-      <c r="G44" s="46" t="n"/>
+      <c r="G44" s="52" t="n"/>
       <c r="H44" s="15" t="n"/>
     </row>
     <row r="45">
@@ -6222,12 +6274,12 @@
   </mergeCells>
   <pageMargins left="0.5299999713897705" right="0.5299999713897705" top="0.5299999713897705" bottom="0.6899999976158142" header="0" footer="0"/>
   <pageSetup orientation="landscape" paperSize="9" scale="0" fitToHeight="0" fitToWidth="0" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6253,32 +6305,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>PLANILHA ORÇAMENTÁRIA</t>
         </is>
       </c>
-      <c r="B1" s="32" t="n"/>
-      <c r="C1" s="32" t="n"/>
-      <c r="D1" s="32" t="n"/>
-      <c r="E1" s="32" t="n"/>
-      <c r="F1" s="32" t="n"/>
-      <c r="G1" s="32" t="n"/>
-      <c r="H1" s="33" t="n"/>
+      <c r="B1" s="36" t="n"/>
+      <c r="C1" s="36" t="n"/>
+      <c r="D1" s="36" t="n"/>
+      <c r="E1" s="36" t="n"/>
+      <c r="F1" s="36" t="n"/>
+      <c r="G1" s="36" t="n"/>
+      <c r="H1" s="37" t="n"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="34" t="n"/>
-      <c r="H2" s="35" t="n"/>
+      <c r="A2" s="38" t="n"/>
+      <c r="H2" s="39" t="n"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="36" t="n"/>
-      <c r="B3" s="37" t="n"/>
-      <c r="C3" s="37" t="n"/>
-      <c r="D3" s="37" t="n"/>
-      <c r="E3" s="37" t="n"/>
-      <c r="F3" s="37" t="n"/>
-      <c r="G3" s="37" t="n"/>
-      <c r="H3" s="38" t="n"/>
+      <c r="A3" s="40" t="n"/>
+      <c r="B3" s="41" t="n"/>
+      <c r="C3" s="41" t="n"/>
+      <c r="D3" s="41" t="n"/>
+      <c r="E3" s="41" t="n"/>
+      <c r="F3" s="41" t="n"/>
+      <c r="G3" s="41" t="n"/>
+      <c r="H3" s="42" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
@@ -6336,7 +6388,7 @@
       <c r="E8" s="8" t="n"/>
       <c r="F8" s="8" t="n"/>
       <c r="G8" s="8" t="n"/>
-      <c r="H8" s="39" t="n"/>
+      <c r="H8" s="43" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
@@ -6346,7 +6398,7 @@
       <c r="E9" s="8" t="n"/>
       <c r="F9" s="8" t="n"/>
       <c r="G9" s="8" t="n"/>
-      <c r="H9" s="39" t="n"/>
+      <c r="H9" s="43" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="21" t="n"/>
@@ -6401,7 +6453,7 @@
       <c r="E12" s="10" t="n"/>
       <c r="F12" s="10" t="n"/>
       <c r="G12" s="10" t="n"/>
-      <c r="H12" s="40" t="n"/>
+      <c r="H12" s="46" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="20" t="n"/>
@@ -6420,8 +6472,8 @@
       <c r="D14" s="10" t="n"/>
       <c r="E14" s="10" t="n"/>
       <c r="F14" s="10" t="n"/>
-      <c r="G14" s="41" t="n"/>
-      <c r="H14" s="42" t="n"/>
+      <c r="G14" s="47" t="n"/>
+      <c r="H14" s="48" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="n"/>
@@ -6430,7 +6482,7 @@
       <c r="D15" s="10" t="n"/>
       <c r="E15" s="10" t="n"/>
       <c r="F15" s="10" t="n"/>
-      <c r="G15" s="43" t="n"/>
+      <c r="G15" s="49" t="n"/>
       <c r="H15" s="15" t="n"/>
     </row>
     <row r="16">
@@ -6441,7 +6493,7 @@
       <c r="E16" s="10" t="n"/>
       <c r="F16" s="10" t="n"/>
       <c r="G16" s="10" t="n"/>
-      <c r="H16" s="44" t="n"/>
+      <c r="H16" s="50" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="9" t="n"/>
@@ -6450,7 +6502,7 @@
       <c r="D17" s="10" t="n"/>
       <c r="E17" s="10" t="n"/>
       <c r="F17" s="10" t="n"/>
-      <c r="G17" s="45" t="n"/>
+      <c r="G17" s="51" t="n"/>
       <c r="H17" s="15" t="n"/>
     </row>
     <row r="18">
@@ -6460,7 +6512,7 @@
       <c r="D18" s="10" t="n"/>
       <c r="E18" s="10" t="n"/>
       <c r="F18" s="10" t="n"/>
-      <c r="G18" s="41" t="n"/>
+      <c r="G18" s="47" t="n"/>
       <c r="H18" s="15" t="n"/>
     </row>
     <row r="19">
@@ -6470,7 +6522,7 @@
       <c r="D19" s="10" t="n"/>
       <c r="E19" s="10" t="n"/>
       <c r="F19" s="10" t="n"/>
-      <c r="G19" s="43" t="n"/>
+      <c r="G19" s="49" t="n"/>
       <c r="H19" s="15" t="n"/>
     </row>
     <row r="20">
@@ -6480,7 +6532,7 @@
       <c r="D20" s="10" t="n"/>
       <c r="E20" s="10" t="n"/>
       <c r="F20" s="10" t="n"/>
-      <c r="G20" s="43" t="n"/>
+      <c r="G20" s="49" t="n"/>
       <c r="H20" s="15" t="n"/>
     </row>
     <row r="21">
@@ -6489,8 +6541,8 @@
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="10" t="n"/>
       <c r="E21" s="10" t="n"/>
-      <c r="F21" s="46" t="n"/>
-      <c r="G21" s="46" t="n"/>
+      <c r="F21" s="52" t="n"/>
+      <c r="G21" s="52" t="n"/>
       <c r="H21" s="15" t="n"/>
     </row>
     <row r="22">
@@ -6501,7 +6553,7 @@
       <c r="E22" s="10" t="n"/>
       <c r="F22" s="10" t="n"/>
       <c r="G22" s="10" t="n"/>
-      <c r="H22" s="44" t="n"/>
+      <c r="H22" s="50" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="9" t="n"/>
@@ -6511,7 +6563,7 @@
       <c r="E23" s="10" t="n"/>
       <c r="F23" s="10" t="n"/>
       <c r="G23" s="10" t="n"/>
-      <c r="H23" s="44" t="n"/>
+      <c r="H23" s="50" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="9" t="n"/>
@@ -6520,18 +6572,18 @@
       <c r="D24" s="10" t="n"/>
       <c r="E24" s="10" t="n"/>
       <c r="F24" s="10" t="n"/>
-      <c r="G24" s="41" t="n"/>
-      <c r="H24" s="44" t="n"/>
+      <c r="G24" s="47" t="n"/>
+      <c r="H24" s="50" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
       <c r="D25" s="10" t="n"/>
-      <c r="E25" s="45" t="n"/>
-      <c r="F25" s="45" t="n"/>
-      <c r="G25" s="45" t="n"/>
-      <c r="H25" s="42" t="n"/>
+      <c r="E25" s="51" t="n"/>
+      <c r="F25" s="51" t="n"/>
+      <c r="G25" s="51" t="n"/>
+      <c r="H25" s="48" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="9" t="n"/>
@@ -6540,7 +6592,7 @@
       <c r="D26" s="10" t="n"/>
       <c r="E26" s="10" t="n"/>
       <c r="F26" s="10" t="n"/>
-      <c r="G26" s="41" t="n"/>
+      <c r="G26" s="47" t="n"/>
       <c r="H26" s="15" t="n"/>
     </row>
     <row r="27">
@@ -6550,7 +6602,7 @@
       <c r="D27" s="10" t="n"/>
       <c r="E27" s="10" t="n"/>
       <c r="F27" s="10" t="n"/>
-      <c r="G27" s="41" t="n"/>
+      <c r="G27" s="47" t="n"/>
       <c r="H27" s="15" t="n"/>
     </row>
     <row r="28">
@@ -6560,7 +6612,7 @@
       <c r="D28" s="10" t="n"/>
       <c r="E28" s="10" t="n"/>
       <c r="F28" s="10" t="n"/>
-      <c r="G28" s="41" t="n"/>
+      <c r="G28" s="47" t="n"/>
       <c r="H28" s="15" t="n"/>
     </row>
     <row r="29">
@@ -6569,8 +6621,8 @@
       <c r="C29" s="9" t="n"/>
       <c r="D29" s="10" t="n"/>
       <c r="E29" s="10" t="n"/>
-      <c r="F29" s="41" t="n"/>
-      <c r="G29" s="41" t="n"/>
+      <c r="F29" s="47" t="n"/>
+      <c r="G29" s="47" t="n"/>
       <c r="H29" s="15" t="n"/>
     </row>
     <row r="30">
@@ -6579,9 +6631,9 @@
       <c r="C30" s="9" t="n"/>
       <c r="D30" s="10" t="n"/>
       <c r="E30" s="10" t="n"/>
-      <c r="F30" s="41" t="n"/>
-      <c r="G30" s="41" t="n"/>
-      <c r="H30" s="44" t="n"/>
+      <c r="F30" s="47" t="n"/>
+      <c r="G30" s="47" t="n"/>
+      <c r="H30" s="50" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="9" t="n"/>
@@ -6590,7 +6642,7 @@
       <c r="D31" s="10" t="n"/>
       <c r="E31" s="10" t="n"/>
       <c r="F31" s="10" t="n"/>
-      <c r="G31" s="41" t="n"/>
+      <c r="G31" s="47" t="n"/>
       <c r="H31" s="15" t="n"/>
     </row>
     <row r="32">
@@ -6600,7 +6652,7 @@
       <c r="D32" s="10" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
-      <c r="G32" s="41" t="n"/>
+      <c r="G32" s="47" t="n"/>
       <c r="H32" s="15" t="n"/>
     </row>
     <row r="33">
@@ -6611,7 +6663,7 @@
       <c r="E33" s="10" t="n"/>
       <c r="F33" s="10" t="n"/>
       <c r="G33" s="10" t="n"/>
-      <c r="H33" s="44" t="n"/>
+      <c r="H33" s="50" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="9" t="n"/>
@@ -6620,17 +6672,17 @@
       <c r="D34" s="10" t="n"/>
       <c r="E34" s="10" t="n"/>
       <c r="F34" s="10" t="n"/>
-      <c r="G34" s="43" t="n"/>
-      <c r="H34" s="42" t="n"/>
+      <c r="G34" s="49" t="n"/>
+      <c r="H34" s="48" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="9" t="n"/>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="9" t="n"/>
       <c r="D35" s="10" t="n"/>
-      <c r="E35" s="43" t="n"/>
+      <c r="E35" s="49" t="n"/>
       <c r="F35" s="10" t="n"/>
-      <c r="G35" s="43" t="n"/>
+      <c r="G35" s="49" t="n"/>
       <c r="H35" s="15" t="n"/>
     </row>
     <row r="36">
@@ -6638,9 +6690,9 @@
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
       <c r="D36" s="10" t="n"/>
-      <c r="E36" s="46" t="n"/>
+      <c r="E36" s="52" t="n"/>
       <c r="F36" s="10" t="n"/>
-      <c r="G36" s="46" t="n"/>
+      <c r="G36" s="52" t="n"/>
       <c r="H36" s="15" t="n"/>
     </row>
     <row r="37">
@@ -6650,7 +6702,7 @@
       <c r="D37" s="10" t="n"/>
       <c r="E37" s="10" t="n"/>
       <c r="F37" s="10" t="n"/>
-      <c r="G37" s="46" t="n"/>
+      <c r="G37" s="52" t="n"/>
       <c r="H37" s="15" t="n"/>
     </row>
     <row r="38">
@@ -6660,27 +6712,27 @@
       <c r="D38" s="10" t="n"/>
       <c r="E38" s="10" t="n"/>
       <c r="F38" s="10" t="n"/>
-      <c r="G38" s="43" t="n"/>
-      <c r="H38" s="42" t="n"/>
+      <c r="G38" s="49" t="n"/>
+      <c r="H38" s="48" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="9" t="n"/>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="9" t="n"/>
       <c r="D39" s="10" t="n"/>
-      <c r="E39" s="43" t="n"/>
-      <c r="F39" s="43" t="n"/>
-      <c r="G39" s="43" t="n"/>
-      <c r="H39" s="42" t="n"/>
+      <c r="E39" s="49" t="n"/>
+      <c r="F39" s="49" t="n"/>
+      <c r="G39" s="49" t="n"/>
+      <c r="H39" s="48" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="9" t="n"/>
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="9" t="n"/>
       <c r="D40" s="10" t="n"/>
-      <c r="E40" s="46" t="n"/>
+      <c r="E40" s="52" t="n"/>
       <c r="F40" s="10" t="n"/>
-      <c r="G40" s="46" t="n"/>
+      <c r="G40" s="52" t="n"/>
       <c r="H40" s="15" t="n"/>
     </row>
     <row r="41">
@@ -6691,7 +6743,7 @@
       <c r="E41" s="10" t="n"/>
       <c r="F41" s="10" t="n"/>
       <c r="G41" s="10" t="n"/>
-      <c r="H41" s="44" t="n"/>
+      <c r="H41" s="50" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="9" t="n"/>
@@ -6700,8 +6752,8 @@
       <c r="D42" s="10" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
-      <c r="G42" s="46" t="n"/>
-      <c r="H42" s="44" t="n"/>
+      <c r="G42" s="52" t="n"/>
+      <c r="H42" s="50" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="9" t="n"/>
@@ -6710,8 +6762,8 @@
       <c r="D43" s="10" t="n"/>
       <c r="E43" s="10" t="n"/>
       <c r="F43" s="10" t="n"/>
-      <c r="G43" s="41" t="n"/>
-      <c r="H43" s="42" t="n"/>
+      <c r="G43" s="47" t="n"/>
+      <c r="H43" s="48" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="9" t="n"/>
@@ -6720,7 +6772,7 @@
       <c r="D44" s="10" t="n"/>
       <c r="E44" s="10" t="n"/>
       <c r="F44" s="10" t="n"/>
-      <c r="G44" s="46" t="n"/>
+      <c r="G44" s="52" t="n"/>
       <c r="H44" s="15" t="n"/>
     </row>
     <row r="45">
@@ -7820,12 +7872,12 @@
   </mergeCells>
   <pageMargins left="0.5299999713897705" right="0.5299999713897705" top="0.5299999713897705" bottom="0.6899999976158142" header="0" footer="0"/>
   <pageSetup orientation="landscape" paperSize="9" scale="0" fitToHeight="0" fitToWidth="0" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -7851,32 +7903,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>PLANILHA ORÇAMENTÁRIA</t>
         </is>
       </c>
-      <c r="B1" s="32" t="n"/>
-      <c r="C1" s="32" t="n"/>
-      <c r="D1" s="32" t="n"/>
-      <c r="E1" s="32" t="n"/>
-      <c r="F1" s="32" t="n"/>
-      <c r="G1" s="32" t="n"/>
-      <c r="H1" s="33" t="n"/>
+      <c r="B1" s="36" t="n"/>
+      <c r="C1" s="36" t="n"/>
+      <c r="D1" s="36" t="n"/>
+      <c r="E1" s="36" t="n"/>
+      <c r="F1" s="36" t="n"/>
+      <c r="G1" s="36" t="n"/>
+      <c r="H1" s="37" t="n"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="34" t="n"/>
-      <c r="H2" s="35" t="n"/>
+      <c r="A2" s="38" t="n"/>
+      <c r="H2" s="39" t="n"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="36" t="n"/>
-      <c r="B3" s="37" t="n"/>
-      <c r="C3" s="37" t="n"/>
-      <c r="D3" s="37" t="n"/>
-      <c r="E3" s="37" t="n"/>
-      <c r="F3" s="37" t="n"/>
-      <c r="G3" s="37" t="n"/>
-      <c r="H3" s="38" t="n"/>
+      <c r="A3" s="40" t="n"/>
+      <c r="B3" s="41" t="n"/>
+      <c r="C3" s="41" t="n"/>
+      <c r="D3" s="41" t="n"/>
+      <c r="E3" s="41" t="n"/>
+      <c r="F3" s="41" t="n"/>
+      <c r="G3" s="41" t="n"/>
+      <c r="H3" s="42" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
@@ -7934,7 +7986,7 @@
       <c r="E8" s="8" t="n"/>
       <c r="F8" s="8" t="n"/>
       <c r="G8" s="8" t="n"/>
-      <c r="H8" s="39" t="n"/>
+      <c r="H8" s="43" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
@@ -7944,7 +7996,7 @@
       <c r="E9" s="8" t="n"/>
       <c r="F9" s="8" t="n"/>
       <c r="G9" s="8" t="n"/>
-      <c r="H9" s="39" t="n"/>
+      <c r="H9" s="43" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="21" t="n"/>
@@ -7999,7 +8051,7 @@
       <c r="E12" s="10" t="n"/>
       <c r="F12" s="10" t="n"/>
       <c r="G12" s="10" t="n"/>
-      <c r="H12" s="40" t="n"/>
+      <c r="H12" s="46" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="20" t="n"/>
@@ -8018,8 +8070,8 @@
       <c r="D14" s="10" t="n"/>
       <c r="E14" s="10" t="n"/>
       <c r="F14" s="10" t="n"/>
-      <c r="G14" s="41" t="n"/>
-      <c r="H14" s="42" t="n"/>
+      <c r="G14" s="47" t="n"/>
+      <c r="H14" s="48" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="n"/>
@@ -8028,7 +8080,7 @@
       <c r="D15" s="10" t="n"/>
       <c r="E15" s="10" t="n"/>
       <c r="F15" s="10" t="n"/>
-      <c r="G15" s="43" t="n"/>
+      <c r="G15" s="49" t="n"/>
       <c r="H15" s="15" t="n"/>
     </row>
     <row r="16">
@@ -8039,7 +8091,7 @@
       <c r="E16" s="10" t="n"/>
       <c r="F16" s="10" t="n"/>
       <c r="G16" s="10" t="n"/>
-      <c r="H16" s="44" t="n"/>
+      <c r="H16" s="50" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="9" t="n"/>
@@ -8048,7 +8100,7 @@
       <c r="D17" s="10" t="n"/>
       <c r="E17" s="10" t="n"/>
       <c r="F17" s="10" t="n"/>
-      <c r="G17" s="45" t="n"/>
+      <c r="G17" s="51" t="n"/>
       <c r="H17" s="15" t="n"/>
     </row>
     <row r="18">
@@ -8058,7 +8110,7 @@
       <c r="D18" s="10" t="n"/>
       <c r="E18" s="10" t="n"/>
       <c r="F18" s="10" t="n"/>
-      <c r="G18" s="41" t="n"/>
+      <c r="G18" s="47" t="n"/>
       <c r="H18" s="15" t="n"/>
     </row>
     <row r="19">
@@ -8068,7 +8120,7 @@
       <c r="D19" s="10" t="n"/>
       <c r="E19" s="10" t="n"/>
       <c r="F19" s="10" t="n"/>
-      <c r="G19" s="43" t="n"/>
+      <c r="G19" s="49" t="n"/>
       <c r="H19" s="15" t="n"/>
     </row>
     <row r="20">
@@ -8078,7 +8130,7 @@
       <c r="D20" s="10" t="n"/>
       <c r="E20" s="10" t="n"/>
       <c r="F20" s="10" t="n"/>
-      <c r="G20" s="43" t="n"/>
+      <c r="G20" s="49" t="n"/>
       <c r="H20" s="15" t="n"/>
     </row>
     <row r="21">
@@ -8087,8 +8139,8 @@
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="10" t="n"/>
       <c r="E21" s="10" t="n"/>
-      <c r="F21" s="46" t="n"/>
-      <c r="G21" s="46" t="n"/>
+      <c r="F21" s="52" t="n"/>
+      <c r="G21" s="52" t="n"/>
       <c r="H21" s="15" t="n"/>
     </row>
     <row r="22">
@@ -8099,7 +8151,7 @@
       <c r="E22" s="10" t="n"/>
       <c r="F22" s="10" t="n"/>
       <c r="G22" s="10" t="n"/>
-      <c r="H22" s="44" t="n"/>
+      <c r="H22" s="50" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="9" t="n"/>
@@ -8109,7 +8161,7 @@
       <c r="E23" s="10" t="n"/>
       <c r="F23" s="10" t="n"/>
       <c r="G23" s="10" t="n"/>
-      <c r="H23" s="44" t="n"/>
+      <c r="H23" s="50" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="9" t="n"/>
@@ -8118,18 +8170,18 @@
       <c r="D24" s="10" t="n"/>
       <c r="E24" s="10" t="n"/>
       <c r="F24" s="10" t="n"/>
-      <c r="G24" s="41" t="n"/>
-      <c r="H24" s="44" t="n"/>
+      <c r="G24" s="47" t="n"/>
+      <c r="H24" s="50" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
       <c r="D25" s="10" t="n"/>
-      <c r="E25" s="45" t="n"/>
-      <c r="F25" s="45" t="n"/>
-      <c r="G25" s="45" t="n"/>
-      <c r="H25" s="42" t="n"/>
+      <c r="E25" s="51" t="n"/>
+      <c r="F25" s="51" t="n"/>
+      <c r="G25" s="51" t="n"/>
+      <c r="H25" s="48" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="9" t="n"/>
@@ -8138,7 +8190,7 @@
       <c r="D26" s="10" t="n"/>
       <c r="E26" s="10" t="n"/>
       <c r="F26" s="10" t="n"/>
-      <c r="G26" s="41" t="n"/>
+      <c r="G26" s="47" t="n"/>
       <c r="H26" s="15" t="n"/>
     </row>
     <row r="27">
@@ -8148,7 +8200,7 @@
       <c r="D27" s="10" t="n"/>
       <c r="E27" s="10" t="n"/>
       <c r="F27" s="10" t="n"/>
-      <c r="G27" s="41" t="n"/>
+      <c r="G27" s="47" t="n"/>
       <c r="H27" s="15" t="n"/>
     </row>
     <row r="28">
@@ -8158,7 +8210,7 @@
       <c r="D28" s="10" t="n"/>
       <c r="E28" s="10" t="n"/>
       <c r="F28" s="10" t="n"/>
-      <c r="G28" s="41" t="n"/>
+      <c r="G28" s="47" t="n"/>
       <c r="H28" s="15" t="n"/>
     </row>
     <row r="29">
@@ -8167,8 +8219,8 @@
       <c r="C29" s="9" t="n"/>
       <c r="D29" s="10" t="n"/>
       <c r="E29" s="10" t="n"/>
-      <c r="F29" s="41" t="n"/>
-      <c r="G29" s="41" t="n"/>
+      <c r="F29" s="47" t="n"/>
+      <c r="G29" s="47" t="n"/>
       <c r="H29" s="15" t="n"/>
     </row>
     <row r="30">
@@ -8177,9 +8229,9 @@
       <c r="C30" s="9" t="n"/>
       <c r="D30" s="10" t="n"/>
       <c r="E30" s="10" t="n"/>
-      <c r="F30" s="41" t="n"/>
-      <c r="G30" s="41" t="n"/>
-      <c r="H30" s="44" t="n"/>
+      <c r="F30" s="47" t="n"/>
+      <c r="G30" s="47" t="n"/>
+      <c r="H30" s="50" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="9" t="n"/>
@@ -8188,7 +8240,7 @@
       <c r="D31" s="10" t="n"/>
       <c r="E31" s="10" t="n"/>
       <c r="F31" s="10" t="n"/>
-      <c r="G31" s="41" t="n"/>
+      <c r="G31" s="47" t="n"/>
       <c r="H31" s="15" t="n"/>
     </row>
     <row r="32">
@@ -8198,7 +8250,7 @@
       <c r="D32" s="10" t="n"/>
       <c r="E32" s="10" t="n"/>
       <c r="F32" s="10" t="n"/>
-      <c r="G32" s="41" t="n"/>
+      <c r="G32" s="47" t="n"/>
       <c r="H32" s="15" t="n"/>
     </row>
     <row r="33">
@@ -8209,7 +8261,7 @@
       <c r="E33" s="10" t="n"/>
       <c r="F33" s="10" t="n"/>
       <c r="G33" s="10" t="n"/>
-      <c r="H33" s="44" t="n"/>
+      <c r="H33" s="50" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="9" t="n"/>
@@ -8218,17 +8270,17 @@
       <c r="D34" s="10" t="n"/>
       <c r="E34" s="10" t="n"/>
       <c r="F34" s="10" t="n"/>
-      <c r="G34" s="43" t="n"/>
-      <c r="H34" s="42" t="n"/>
+      <c r="G34" s="49" t="n"/>
+      <c r="H34" s="48" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="9" t="n"/>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="9" t="n"/>
       <c r="D35" s="10" t="n"/>
-      <c r="E35" s="43" t="n"/>
+      <c r="E35" s="49" t="n"/>
       <c r="F35" s="10" t="n"/>
-      <c r="G35" s="43" t="n"/>
+      <c r="G35" s="49" t="n"/>
       <c r="H35" s="15" t="n"/>
     </row>
     <row r="36">
@@ -8236,9 +8288,9 @@
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
       <c r="D36" s="10" t="n"/>
-      <c r="E36" s="46" t="n"/>
+      <c r="E36" s="52" t="n"/>
       <c r="F36" s="10" t="n"/>
-      <c r="G36" s="46" t="n"/>
+      <c r="G36" s="52" t="n"/>
       <c r="H36" s="15" t="n"/>
     </row>
     <row r="37">
@@ -8248,7 +8300,7 @@
       <c r="D37" s="10" t="n"/>
       <c r="E37" s="10" t="n"/>
       <c r="F37" s="10" t="n"/>
-      <c r="G37" s="46" t="n"/>
+      <c r="G37" s="52" t="n"/>
       <c r="H37" s="15" t="n"/>
     </row>
     <row r="38">
@@ -8258,27 +8310,27 @@
       <c r="D38" s="10" t="n"/>
       <c r="E38" s="10" t="n"/>
       <c r="F38" s="10" t="n"/>
-      <c r="G38" s="43" t="n"/>
-      <c r="H38" s="42" t="n"/>
+      <c r="G38" s="49" t="n"/>
+      <c r="H38" s="48" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="9" t="n"/>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="9" t="n"/>
       <c r="D39" s="10" t="n"/>
-      <c r="E39" s="43" t="n"/>
-      <c r="F39" s="43" t="n"/>
-      <c r="G39" s="43" t="n"/>
-      <c r="H39" s="42" t="n"/>
+      <c r="E39" s="49" t="n"/>
+      <c r="F39" s="49" t="n"/>
+      <c r="G39" s="49" t="n"/>
+      <c r="H39" s="48" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="9" t="n"/>
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="9" t="n"/>
       <c r="D40" s="10" t="n"/>
-      <c r="E40" s="46" t="n"/>
+      <c r="E40" s="52" t="n"/>
       <c r="F40" s="10" t="n"/>
-      <c r="G40" s="46" t="n"/>
+      <c r="G40" s="52" t="n"/>
       <c r="H40" s="15" t="n"/>
     </row>
     <row r="41">
@@ -8289,7 +8341,7 @@
       <c r="E41" s="10" t="n"/>
       <c r="F41" s="10" t="n"/>
       <c r="G41" s="10" t="n"/>
-      <c r="H41" s="44" t="n"/>
+      <c r="H41" s="50" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="9" t="n"/>
@@ -8298,8 +8350,8 @@
       <c r="D42" s="10" t="n"/>
       <c r="E42" s="10" t="n"/>
       <c r="F42" s="10" t="n"/>
-      <c r="G42" s="46" t="n"/>
-      <c r="H42" s="44" t="n"/>
+      <c r="G42" s="52" t="n"/>
+      <c r="H42" s="50" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="9" t="n"/>
@@ -8308,8 +8360,8 @@
       <c r="D43" s="10" t="n"/>
       <c r="E43" s="10" t="n"/>
       <c r="F43" s="10" t="n"/>
-      <c r="G43" s="41" t="n"/>
-      <c r="H43" s="42" t="n"/>
+      <c r="G43" s="47" t="n"/>
+      <c r="H43" s="48" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="9" t="n"/>
@@ -8318,7 +8370,7 @@
       <c r="D44" s="10" t="n"/>
       <c r="E44" s="10" t="n"/>
       <c r="F44" s="10" t="n"/>
-      <c r="G44" s="46" t="n"/>
+      <c r="G44" s="52" t="n"/>
       <c r="H44" s="15" t="n"/>
     </row>
     <row r="45">
@@ -9418,6 +9470,6 @@
   </mergeCells>
   <pageMargins left="0.5299999713897705" right="0.5299999713897705" top="0.5299999713897705" bottom="0.6899999976158142" header="0" footer="0"/>
   <pageSetup orientation="landscape" paperSize="9" scale="0" fitToHeight="0" fitToWidth="0" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>